<commit_message>
Correct mistakes and harmonize text
</commit_message>
<xml_diff>
--- a/tables/combination_drugs.xlsx
+++ b/tables/combination_drugs.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="20379"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="24527"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="Z:\lit_review_semi_mechanistic_models\tables\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Vincent\Documents\pmx-models-atb-review\tables\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AD2EBDAB-76D7-48B4-9016-43693D42304B}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FAD05E32-D512-4F7B-ABFF-3486228AB56E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1464" yWindow="1464" windowWidth="17280" windowHeight="8964" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -97,18 +97,12 @@
     <t>Static kill-curves</t>
   </si>
   <si>
-    <t>additivity, decrease in ec50, meropenem, sulbactam, gpdi like</t>
-  </si>
-  <si>
     <t>fosfomycin + sulbactam</t>
   </si>
   <si>
     <t>Acinetobacter baumannii, 4 strains</t>
   </si>
   <si>
-    <t>additivity, decrease in ec50, fosfomycin, sulbactam, gpdi like</t>
-  </si>
-  <si>
     <t>ciprofloxacin + meropenem</t>
   </si>
   <si>
@@ -133,15 +127,9 @@
     <t>Onufrak</t>
   </si>
   <si>
-    <t>additivity, decrease in ec50, polymyxin b, meroepenm, gpdi like</t>
-  </si>
-  <si>
     <t>Inoculum effect</t>
   </si>
   <si>
-    <t>minocycline + polymyxin b</t>
-  </si>
-  <si>
     <t>Zhao</t>
   </si>
   <si>
@@ -151,9 +139,6 @@
     <t>adaptive resistance, NA</t>
   </si>
   <si>
-    <t>additivity, increase in emax, polymyxin b, minocycline, gpdi</t>
-  </si>
-  <si>
     <t>Acinetobacter baumannii, 1 strains</t>
   </si>
   <si>
@@ -163,9 +148,6 @@
     <t>subpopulations, NA;adaptive resistance, NA</t>
   </si>
   <si>
-    <t>additivity, decrease in ec50, polymyxin b, minocycline, gpdi;additivity, decrease in adaptive resistance rate, minocycline, polymyxin b, gpdi</t>
-  </si>
-  <si>
     <t>I don't know the authors personally but it is certainly a very good article</t>
   </si>
   <si>
@@ -181,9 +163,6 @@
     <t>subpopulations, NA;other, beta lacatamases degrading ceftazidime</t>
   </si>
   <si>
-    <t>bliss, decrease in ec50, avibactam, ceftazidime, gpdi like;bliss, decrease in drug degradation rate, avibactam, ceftazidime, NA</t>
-  </si>
-  <si>
     <t>ciprofloxacin + tobramycin</t>
   </si>
   <si>
@@ -193,9 +172,6 @@
     <t>Rees</t>
   </si>
   <si>
-    <t>additivity, decrease in ec50, tobramycin, ciprofloxacin, gpdi like</t>
-  </si>
-  <si>
     <t>imipenem + relebactam</t>
   </si>
   <si>
@@ -208,12 +184,6 @@
     <t>Hollow Fibre kill-curves;Other experiment type</t>
   </si>
   <si>
-    <t>adaptive resistance, not the uppsala way</t>
-  </si>
-  <si>
-    <t>additivity, decrease in ec50, relebactam, imipenem, gpdi like</t>
-  </si>
-  <si>
     <t>avibactam + aztreonam</t>
   </si>
   <si>
@@ -238,18 +208,12 @@
     <t>additivity, power on individual effects, NA, NA, NA</t>
   </si>
   <si>
-    <t>polymyxin b + zidovudine</t>
-  </si>
-  <si>
     <t>Klebsiella pneumoniae, 3 strains</t>
   </si>
   <si>
     <t>Lin</t>
   </si>
   <si>
-    <t>additivity, decrease in ec50, polymyxin b, zidovudine, gpdi like</t>
-  </si>
-  <si>
     <t>colistin + fusidic acid</t>
   </si>
   <si>
@@ -259,9 +223,6 @@
     <t>Phee</t>
   </si>
   <si>
-    <t>additivity, decrease in ec50, fusidic acid, colistin, NA;additivity, increase in emax, colistin, fusidic acid, NA</t>
-  </si>
-  <si>
     <t>quite a bit of data in there !</t>
   </si>
   <si>
@@ -277,27 +238,15 @@
     <t>2 metabolic states</t>
   </si>
   <si>
-    <t>additivity, decrease in ec50, ciprofloxacin, meropenem, gpdi like</t>
-  </si>
-  <si>
-    <t>enrofloxacin + polymyxin b</t>
-  </si>
-  <si>
     <t>Static kill-curves;Dynamic kill-curves;Hollow Fibre kill-curves</t>
   </si>
   <si>
-    <t>additivity, decrease in ec50, polymyxin b, enrofloxacin, gpdi like</t>
-  </si>
-  <si>
     <t>piperacillin + tazobactam</t>
   </si>
   <si>
     <t>Yadav</t>
   </si>
   <si>
-    <t>additivity, decrease in ec50, tobramycin, piperacillin, gpdi like</t>
-  </si>
-  <si>
     <t>meropenem + tobramycin</t>
   </si>
   <si>
@@ -307,21 +256,12 @@
     <t>Landersdorfer</t>
   </si>
   <si>
-    <t>additivity, decrease in ec50, tobramycin, meropenem, gpdi like</t>
-  </si>
-  <si>
     <t>Sy</t>
   </si>
   <si>
     <t>imipenem + tobramycin</t>
   </si>
   <si>
-    <t>additivity, decrease in ec50, tobramycin, imipenem, not a continuous relationship: reduction of imipenem ec50 when tobramaycin concentration is higher than a cutoff</t>
-  </si>
-  <si>
-    <t>additivity, decrease in ec50, tobramycin, imipenem, gpdi like</t>
-  </si>
-  <si>
     <t>In vivo mouse thigh study</t>
   </si>
   <si>
@@ -340,9 +280,6 @@
     <t>3 metabolic states</t>
   </si>
   <si>
-    <t>sEmax, NA, no, linezolid, NA, eagle effect due to meropenem;sEmax, NA, no, meropenem, NA, meropenem eagle effect</t>
-  </si>
-  <si>
     <t>Escherichia coli, 2 strains;Klebsiella pneumoniae, 1 strains;Pseudomonas aeruginosa, 1 strains</t>
   </si>
   <si>
@@ -352,12 +289,6 @@
     <t>subpopulations, NA;other, signal molecules</t>
   </si>
   <si>
-    <t>additivity, decrease in ec50, tobramycin, imipenem, emax equation;additivity, decrease in ec50, amikacin, imipenem, emax equation</t>
-  </si>
-  <si>
-    <t>doripenem + polymyxin b</t>
-  </si>
-  <si>
     <t>Rao</t>
   </si>
   <si>
@@ -382,9 +313,6 @@
     <t>Ly</t>
   </si>
   <si>
-    <t>additivity, decrease in ec50, colistin, doripenem, not a continuous relationship: different doripenem ec50 values for discrete colistin concentrations</t>
-  </si>
-  <si>
     <t>Population analysis profiles were also performed, cation displacement model for colistin available concentration</t>
   </si>
   <si>
@@ -409,9 +337,6 @@
     <t>mouse infection model</t>
   </si>
   <si>
-    <t>amikacin + nisin a;linezolid + nisin a</t>
-  </si>
-  <si>
     <t>Escherichia coli, 1 strains;Staphylococcus aureus, 1 strains</t>
   </si>
   <si>
@@ -424,21 +349,12 @@
     <t>Pseudomonas aeruginosa, 6 strains</t>
   </si>
   <si>
-    <t>Emax, death, no, doripenem, NA, NA;linear, death, no, polymyxin b, NA, NA</t>
-  </si>
-  <si>
     <t>subpopualations, NA</t>
   </si>
   <si>
-    <t>additivity, increase in emax, polymyxin b, doripenem, only on doripenem susceptible subpopulation</t>
-  </si>
-  <si>
     <t>https://www.ncbi.nlm.nih.gov/pmc/articles/PMC4862466/pdf/zac2870.pdf</t>
   </si>
   <si>
-    <t>meropenem + polymyxin b</t>
-  </si>
-  <si>
     <t>Lenhard</t>
   </si>
   <si>
@@ -448,9 +364,6 @@
     <t>subpopualations, NA;other, signal molecules</t>
   </si>
   <si>
-    <t>additivity, decrease in ec50, polymyxin b, meropenem, threshold of polymyxin b concentration above which ec50 of meropenem decreases</t>
-  </si>
-  <si>
     <t>https://academic.oup.com/jac/article/72/1/153/2643127</t>
   </si>
   <si>
@@ -460,9 +373,6 @@
     <t>No resistance model, NA</t>
   </si>
   <si>
-    <t>greco ursa model, greco ursa interaction parameter, NA, NA, NA</t>
-  </si>
-  <si>
     <t>additivity, no interaction parameter, NA, NA, NA</t>
   </si>
   <si>
@@ -478,9 +388,6 @@
     <t>critically ill with arc, simulations;critically ill with arc, experimental setup</t>
   </si>
   <si>
-    <t>no pk population</t>
-  </si>
-  <si>
     <t>cystic fibrosis patients, simulations</t>
   </si>
   <si>
@@ -508,9 +415,6 @@
     <t>critically ill patients, experimental setup</t>
   </si>
   <si>
-    <t>general patient pop with 5% chance of liver cirrhosis, simulations</t>
-  </si>
-  <si>
     <t>critically ill patients, simulations</t>
   </si>
   <si>
@@ -535,9 +439,6 @@
     <t>lag time on transfer from growing to resting</t>
   </si>
   <si>
-    <t>Emax, death, no, minocycline, NA, NA;linear-power, death, no, polymyxin b, NA, NA</t>
-  </si>
-  <si>
     <t>Emax, death, yes, NA, NA, NA</t>
   </si>
   <si>
@@ -547,9 +448,6 @@
     <t>1 metabolic state, emax growth, no delay</t>
   </si>
   <si>
-    <t>sEmax, growth, no, zidovudine, NA, NA;sEmax, death, no, polymyxin b, NA, NA</t>
-  </si>
-  <si>
     <t>1 metabolic state, logistic growth, delay</t>
   </si>
   <si>
@@ -571,18 +469,12 @@
     <t>Animal experiments</t>
   </si>
   <si>
-    <t>sEmax, death, no, imipenem, NA, NA;none, NA, no, tobramycin, NA, NA</t>
-  </si>
-  <si>
     <t>3 metabolic states (2 life cycle model with persisters), NA, delay</t>
   </si>
   <si>
     <t>sEmax, death, no, aztreonam, NA, growth delay due to drug</t>
   </si>
   <si>
-    <t>linear, death, no, polymyxin b, NA, NA;Emax, death, no, doripenem, NA, NA</t>
-  </si>
-  <si>
     <t>sEmax, death, no, meropenem, NA, resistant strain;Emax, death, no, colistin, NA, susceptible strain;linear, death, no, colistin, NA, resistant strain;linear-power, death, no, meropenem, NA, susceptible strain</t>
   </si>
   <si>
@@ -601,12 +493,6 @@
     <t>ciprofloxacin + gentamicin;ciprofloxacin + oxacillin;ciprofloxacin + vancomycin;gentamicin + oxacillin;gentamicin + vancomycin;oxacillin + vancomycin;ampicillin + ciprofloxacin;ciprofloxacin + tetracycline;ciprofloxacin + tobramycin;ampicillin + tetracycline;ampicillin + tobramycin;tetracycline + tobramycin</t>
   </si>
   <si>
-    <t>meropenem + polymyxin b + rifampicin</t>
-  </si>
-  <si>
-    <t>Emax, NA, no, meropenem, NA, NA;Emax, NA, no, rifampicin, NA, NA;linear, NA, no, polymyxin b, NA, NA</t>
-  </si>
-  <si>
     <t>loewe additivity, no interaction parameter, NA, NA, NA</t>
   </si>
   <si>
@@ -616,15 +502,6 @@
     <t>linear power, death, no, NA, NA, NA</t>
   </si>
   <si>
-    <t>additivity, decrease in ec50, avibactam, aztreonam, biexponential equation of aztronam ec50 dependent on avibactam concentrations;additivity, decrease in drug degradation rate, avibactam, aztreonam, NA</t>
-  </si>
-  <si>
-    <t>additivity, decrease in ec50, avibactam, ceftazidime, biexponential equation of ceftazidime ec50 dependent on avibactam concentrations;additivity, decrease in drug degradation rate, avibactam, ceftazidime, NA</t>
-  </si>
-  <si>
-    <t>additivity, decrease in ec50, avibactam, aztreonam, biexponential equation of aztronam ec50 dependent on avibactam concentrations</t>
-  </si>
-  <si>
     <t>Escherichia coli</t>
   </si>
   <si>
@@ -649,7 +526,130 @@
     <t>sEmax, death, no, meropenem, NA, NA;linear, death, no, polymyxin B, NA, NA</t>
   </si>
   <si>
-    <t>additivity, decrease in ec50, polymyxin b, meropenem, reduction of growth rate by polymyxin b</t>
+    <t>-</t>
+  </si>
+  <si>
+    <t>greco ursa model, greco interaction model, NA, NA, NA</t>
+  </si>
+  <si>
+    <t>amikacin + nisin A;linezolid + nisin A</t>
+  </si>
+  <si>
+    <t>doripenem + polymyxin B</t>
+  </si>
+  <si>
+    <t>additivity, increase in Emax, polymyxin B, doripenem, only on doripenem susceptible subpopulation</t>
+  </si>
+  <si>
+    <t>meropenem + polymyxin B + rifampicin</t>
+  </si>
+  <si>
+    <t>Emax, NA, no, meropenem, NA, NA;Emax, NA, no, rifampicin, NA, NA;linear, NA, no, polymyxin B, NA, NA</t>
+  </si>
+  <si>
+    <t>minocycline + polymyxin B</t>
+  </si>
+  <si>
+    <t>Emax, death, no, minocycline, NA, NA;linear-power, death, no, polymyxin B, NA, NA</t>
+  </si>
+  <si>
+    <t>polymyxin B + zidovudine</t>
+  </si>
+  <si>
+    <t>sEmax, growth, no, zidovudine, NA, NA;sEmax, death, no, polymyxin B, NA, NA</t>
+  </si>
+  <si>
+    <t>enrofloxacin + polymyxin B</t>
+  </si>
+  <si>
+    <t>linear, death, no, polymyxin B, NA, NA;Emax, death, no, doripenem, NA, NA</t>
+  </si>
+  <si>
+    <t>Emax, death, no, doripenem, NA, NA;linear, death, no, polymyxin B, NA, NA</t>
+  </si>
+  <si>
+    <t>meropenem + polymyxin B</t>
+  </si>
+  <si>
+    <t>additivity, decrease in EC50, polymyxin B, meropenem, threshold of polymyxin B concentration above which EC50 of meropenem decreases</t>
+  </si>
+  <si>
+    <t>additivity, decrease in EC50, avibactam, aztreonam, biexponential equation of aztronam EC50 dependent on avibactam concentrations;additivity, decrease in drug degradation rate, avibactam, aztreonam, NA</t>
+  </si>
+  <si>
+    <t>additivity, decrease in EC50, fusidic acid, colistin, NA;additivity, increase in emax, colistin, fusidic acid, NA</t>
+  </si>
+  <si>
+    <t>additivity, decrease in EC50, avibactam, ceftazidime, biexponential equation of ceftazidime EC50 dependent on avibactam concentrations;additivity, decrease in drug degradation rate, avibactam, ceftazidime, NA</t>
+  </si>
+  <si>
+    <t>additivity, decrease in EC50, tobramycin, imipenem, emax equation;additivity, decrease in EC50, amikacin, imipenem, emax equation</t>
+  </si>
+  <si>
+    <t>additivity, decrease in EC50, colistin, doripenem, not a continuous relationship: different doripenem EC50 values for discrete colistin concentrations</t>
+  </si>
+  <si>
+    <t>additivity, decrease in EC50, polymyxin B, meropenem, reduction of growth rate by polymyxin B</t>
+  </si>
+  <si>
+    <t>sEmax, death, no, imipenem, NA, NA</t>
+  </si>
+  <si>
+    <t>general patient population with 5% chance of liver cirrhosis, simulations</t>
+  </si>
+  <si>
+    <t>sEmax, NA, no, linezolid, NA, Eagle effect due to meropenem;sEmax, NA, no, meropenem, NA, meropenem eagle effect</t>
+  </si>
+  <si>
+    <t>additivity, decrease in EC50, avibactam, aztreonam, biexponential equation of aztreonam EC50 dependent on avibactam concentrations</t>
+  </si>
+  <si>
+    <t>2 state life cycle model</t>
+  </si>
+  <si>
+    <t>additivity, decrease in EC50, tobramycin, imipenem, not a continuous relationship: reduction of imipenem EC50 when tobramycin concentration is higher than a cutoff</t>
+  </si>
+  <si>
+    <t>additivity, decrease in EC50, meropenem, sulbactam, GPDI like</t>
+  </si>
+  <si>
+    <t>additivity, decrease in EC50, fosfomycin, sulbactam, GPDI like</t>
+  </si>
+  <si>
+    <t>additivity, decrease in EC50, polymyxin B, meroepenm, GPDI like</t>
+  </si>
+  <si>
+    <t>additivity, increase in emax, polymyxin B, minocycline, GPDI</t>
+  </si>
+  <si>
+    <t>additivity, decrease in EC50, polymyxin B, minocycline, GPDI;additivity, decrease in adaptive resistance rate, minocycline, polymyxin B, GPDI</t>
+  </si>
+  <si>
+    <t>bliss, decrease in EC50, avibactam, ceftazidime, GPDI like;bliss, decrease in drug degradation rate, avibactam, ceftazidime, NA</t>
+  </si>
+  <si>
+    <t>additivity, decrease in EC50, tobramycin, ciprofloxacin, GPDI like</t>
+  </si>
+  <si>
+    <t>additivity, decrease in EC50, relebactam, imipenem, GPDI like</t>
+  </si>
+  <si>
+    <t>additivity, decrease in EC50, polymyxin B, zidovudine, GPDI like</t>
+  </si>
+  <si>
+    <t>additivity, decrease in EC50, ciprofloxacin, meropenem, GPDI like</t>
+  </si>
+  <si>
+    <t>additivity, decrease in EC50, polymyxin B, enrofloxacin, GPDI like</t>
+  </si>
+  <si>
+    <t>additivity, decrease in EC50, tobramycin, piperacillin, GPDI like</t>
+  </si>
+  <si>
+    <t>additivity, decrease in EC50, tobramycin, meropenem, GPDI like</t>
+  </si>
+  <si>
+    <t>additivity, decrease in EC50, tobramycin, imipenem, GPDI like</t>
   </si>
 </sst>
 </file>
@@ -717,7 +717,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Thème Office">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -1039,13 +1039,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:O41"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="R17" sqref="R17"/>
+    <sheetView tabSelected="1" topLeftCell="C7" workbookViewId="0">
+      <selection activeCell="L16" sqref="L16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:15" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:15" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1092,7 +1092,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>15</v>
       </c>
@@ -1112,25 +1112,25 @@
         <v>18</v>
       </c>
       <c r="G2" t="s">
-        <v>166</v>
+        <v>134</v>
       </c>
       <c r="H2" t="s">
         <v>19</v>
       </c>
       <c r="I2" t="s">
-        <v>167</v>
+        <v>135</v>
       </c>
       <c r="J2" t="s">
         <v>20</v>
       </c>
       <c r="K2" t="s">
-        <v>146</v>
+        <v>169</v>
       </c>
       <c r="L2" t="s">
-        <v>149</v>
-      </c>
-    </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="3" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>21</v>
       </c>
@@ -1150,30 +1150,30 @@
         <v>24</v>
       </c>
       <c r="G3" t="s">
-        <v>166</v>
+        <v>134</v>
       </c>
       <c r="H3" t="s">
         <v>19</v>
       </c>
       <c r="I3" t="s">
-        <v>167</v>
+        <v>135</v>
       </c>
       <c r="J3" t="s">
         <v>20</v>
       </c>
       <c r="K3" t="s">
+        <v>196</v>
+      </c>
+      <c r="L3" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="4" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
         <v>25</v>
       </c>
-      <c r="L3" t="s">
-        <v>150</v>
-      </c>
-    </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
+      <c r="B4" t="s">
         <v>26</v>
-      </c>
-      <c r="B4" t="s">
-        <v>27</v>
       </c>
       <c r="C4" t="s">
         <v>23</v>
@@ -1188,33 +1188,33 @@
         <v>24</v>
       </c>
       <c r="G4" t="s">
-        <v>166</v>
+        <v>134</v>
       </c>
       <c r="H4" t="s">
         <v>19</v>
       </c>
       <c r="I4" t="s">
-        <v>167</v>
+        <v>135</v>
       </c>
       <c r="J4" t="s">
         <v>20</v>
       </c>
       <c r="K4" t="s">
+        <v>197</v>
+      </c>
+      <c r="L4" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="5" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>27</v>
+      </c>
+      <c r="B5" t="s">
         <v>28</v>
       </c>
-      <c r="L4" t="s">
-        <v>150</v>
-      </c>
-    </row>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
+      <c r="C5" t="s">
         <v>29</v>
-      </c>
-      <c r="B5" t="s">
-        <v>30</v>
-      </c>
-      <c r="C5" t="s">
-        <v>31</v>
       </c>
       <c r="D5">
         <v>2021</v>
@@ -1223,36 +1223,36 @@
         <v>33550617</v>
       </c>
       <c r="F5" t="s">
+        <v>30</v>
+      </c>
+      <c r="G5" t="s">
+        <v>136</v>
+      </c>
+      <c r="H5" t="s">
+        <v>31</v>
+      </c>
+      <c r="I5" t="s">
         <v>32</v>
-      </c>
-      <c r="G5" t="s">
-        <v>168</v>
-      </c>
-      <c r="H5" t="s">
-        <v>33</v>
-      </c>
-      <c r="I5" t="s">
-        <v>34</v>
       </c>
       <c r="J5" t="s">
         <v>20</v>
       </c>
       <c r="K5" t="s">
-        <v>147</v>
+        <v>117</v>
       </c>
       <c r="L5" t="s">
-        <v>151</v>
-      </c>
-    </row>
-    <row r="6" spans="1:15" x14ac:dyDescent="0.25">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="6" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>193</v>
+        <v>173</v>
       </c>
       <c r="B6" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="C6" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="D6">
         <v>2020</v>
@@ -1264,36 +1264,36 @@
         <v>18</v>
       </c>
       <c r="G6" t="s">
-        <v>168</v>
+        <v>136</v>
       </c>
       <c r="H6" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="I6" t="s">
-        <v>194</v>
+        <v>174</v>
       </c>
       <c r="J6" t="s">
         <v>20</v>
       </c>
       <c r="K6" t="s">
-        <v>37</v>
+        <v>198</v>
       </c>
       <c r="L6" t="s">
-        <v>152</v>
+        <v>168</v>
       </c>
       <c r="M6" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="7" spans="1:15" x14ac:dyDescent="0.25">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="7" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>39</v>
+        <v>175</v>
       </c>
       <c r="B7" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="C7" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="D7">
         <v>2020</v>
@@ -1305,36 +1305,36 @@
         <v>24</v>
       </c>
       <c r="G7" t="s">
-        <v>169</v>
+        <v>137</v>
       </c>
       <c r="H7" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
       <c r="I7" t="s">
-        <v>197</v>
+        <v>159</v>
       </c>
       <c r="J7" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
       <c r="K7" t="s">
-        <v>43</v>
+        <v>199</v>
       </c>
       <c r="L7" t="s">
-        <v>152</v>
+        <v>168</v>
       </c>
       <c r="M7" t="s">
-        <v>170</v>
-      </c>
-    </row>
-    <row r="8" spans="1:15" x14ac:dyDescent="0.25">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="8" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
+        <v>175</v>
+      </c>
+      <c r="B8" t="s">
         <v>39</v>
       </c>
-      <c r="B8" t="s">
-        <v>44</v>
-      </c>
       <c r="C8" t="s">
-        <v>45</v>
+        <v>40</v>
       </c>
       <c r="D8">
         <v>2020</v>
@@ -1346,36 +1346,36 @@
         <v>24</v>
       </c>
       <c r="G8" t="s">
-        <v>166</v>
+        <v>134</v>
       </c>
       <c r="H8" t="s">
         <v>19</v>
       </c>
       <c r="I8" t="s">
-        <v>171</v>
+        <v>176</v>
       </c>
       <c r="J8" t="s">
-        <v>46</v>
+        <v>41</v>
       </c>
       <c r="K8" t="s">
-        <v>47</v>
+        <v>200</v>
       </c>
       <c r="L8" t="s">
-        <v>152</v>
+        <v>168</v>
       </c>
       <c r="N8" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="9" spans="1:15" x14ac:dyDescent="0.25">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="9" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>49</v>
+        <v>43</v>
       </c>
       <c r="B9" t="s">
-        <v>50</v>
+        <v>44</v>
       </c>
       <c r="C9" t="s">
-        <v>51</v>
+        <v>45</v>
       </c>
       <c r="D9">
         <v>2020</v>
@@ -1387,33 +1387,33 @@
         <v>24</v>
       </c>
       <c r="G9" t="s">
-        <v>169</v>
+        <v>137</v>
       </c>
       <c r="H9" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
       <c r="I9" t="s">
-        <v>172</v>
+        <v>139</v>
       </c>
       <c r="J9" t="s">
-        <v>52</v>
+        <v>46</v>
       </c>
       <c r="K9" t="s">
-        <v>53</v>
+        <v>201</v>
       </c>
       <c r="L9" t="s">
-        <v>153</v>
-      </c>
-    </row>
-    <row r="10" spans="1:15" x14ac:dyDescent="0.25">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="10" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>54</v>
+        <v>47</v>
       </c>
       <c r="B10" t="s">
-        <v>55</v>
+        <v>48</v>
       </c>
       <c r="C10" t="s">
-        <v>56</v>
+        <v>49</v>
       </c>
       <c r="D10">
         <v>2019</v>
@@ -1425,33 +1425,33 @@
         <v>24</v>
       </c>
       <c r="G10" t="s">
-        <v>168</v>
+        <v>136</v>
       </c>
       <c r="H10" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="I10" t="s">
-        <v>173</v>
+        <v>140</v>
       </c>
       <c r="J10" t="s">
         <v>20</v>
       </c>
       <c r="K10" t="s">
-        <v>57</v>
+        <v>202</v>
       </c>
       <c r="L10" t="s">
-        <v>152</v>
-      </c>
-    </row>
-    <row r="11" spans="1:15" x14ac:dyDescent="0.25">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="11" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>58</v>
+        <v>50</v>
       </c>
       <c r="B11" t="s">
-        <v>59</v>
+        <v>51</v>
       </c>
       <c r="C11" t="s">
-        <v>60</v>
+        <v>52</v>
       </c>
       <c r="D11">
         <v>2019</v>
@@ -1460,36 +1460,36 @@
         <v>31479762</v>
       </c>
       <c r="F11" t="s">
-        <v>61</v>
+        <v>53</v>
       </c>
       <c r="G11" t="s">
-        <v>169</v>
+        <v>137</v>
       </c>
       <c r="H11" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
       <c r="I11" t="s">
-        <v>167</v>
+        <v>135</v>
       </c>
       <c r="J11" t="s">
-        <v>62</v>
+        <v>38</v>
       </c>
       <c r="K11" t="s">
-        <v>63</v>
+        <v>203</v>
       </c>
       <c r="L11" t="s">
-        <v>154</v>
-      </c>
-    </row>
-    <row r="12" spans="1:15" x14ac:dyDescent="0.25">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="12" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>64</v>
+        <v>54</v>
       </c>
       <c r="B12" t="s">
-        <v>65</v>
+        <v>55</v>
       </c>
       <c r="C12" t="s">
-        <v>66</v>
+        <v>56</v>
       </c>
       <c r="D12">
         <v>2019</v>
@@ -1501,33 +1501,33 @@
         <v>24</v>
       </c>
       <c r="G12" t="s">
-        <v>166</v>
+        <v>134</v>
       </c>
       <c r="H12" t="s">
         <v>19</v>
       </c>
       <c r="I12" t="s">
-        <v>167</v>
+        <v>135</v>
       </c>
       <c r="J12" t="s">
         <v>20</v>
       </c>
       <c r="K12" t="s">
-        <v>198</v>
+        <v>184</v>
       </c>
       <c r="L12" t="s">
-        <v>155</v>
-      </c>
-    </row>
-    <row r="13" spans="1:15" x14ac:dyDescent="0.25">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="13" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>67</v>
+        <v>57</v>
       </c>
       <c r="B13" t="s">
-        <v>68</v>
+        <v>58</v>
       </c>
       <c r="C13" t="s">
-        <v>69</v>
+        <v>59</v>
       </c>
       <c r="D13">
         <v>2019</v>
@@ -1536,36 +1536,36 @@
         <v>30745385</v>
       </c>
       <c r="F13" t="s">
-        <v>70</v>
+        <v>60</v>
       </c>
       <c r="G13" t="s">
-        <v>166</v>
+        <v>134</v>
       </c>
       <c r="H13" t="s">
         <v>19</v>
       </c>
       <c r="I13" t="s">
-        <v>167</v>
+        <v>135</v>
       </c>
       <c r="J13" t="s">
+        <v>38</v>
+      </c>
+      <c r="K13" t="s">
+        <v>61</v>
+      </c>
+      <c r="L13" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="14" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A14" t="s">
+        <v>177</v>
+      </c>
+      <c r="B14" t="s">
         <v>62</v>
       </c>
-      <c r="K13" t="s">
-        <v>71</v>
-      </c>
-      <c r="L13" t="s">
-        <v>154</v>
-      </c>
-    </row>
-    <row r="14" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A14" t="s">
-        <v>72</v>
-      </c>
-      <c r="B14" t="s">
-        <v>73</v>
-      </c>
       <c r="C14" t="s">
-        <v>74</v>
+        <v>63</v>
       </c>
       <c r="D14">
         <v>2019</v>
@@ -1577,33 +1577,33 @@
         <v>24</v>
       </c>
       <c r="G14" t="s">
-        <v>174</v>
+        <v>141</v>
       </c>
       <c r="H14" t="s">
         <v>19</v>
       </c>
       <c r="I14" t="s">
-        <v>175</v>
+        <v>178</v>
       </c>
       <c r="J14" t="s">
         <v>20</v>
       </c>
       <c r="K14" t="s">
-        <v>75</v>
+        <v>204</v>
       </c>
       <c r="L14" t="s">
-        <v>152</v>
-      </c>
-    </row>
-    <row r="15" spans="1:15" x14ac:dyDescent="0.25">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="15" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
-        <v>76</v>
+        <v>64</v>
       </c>
       <c r="B15" t="s">
-        <v>77</v>
+        <v>65</v>
       </c>
       <c r="C15" t="s">
-        <v>78</v>
+        <v>66</v>
       </c>
       <c r="D15">
         <v>2019</v>
@@ -1615,36 +1615,36 @@
         <v>24</v>
       </c>
       <c r="G15" t="s">
-        <v>176</v>
+        <v>142</v>
       </c>
       <c r="H15" t="s">
         <v>19</v>
       </c>
       <c r="I15" t="s">
-        <v>177</v>
+        <v>143</v>
       </c>
       <c r="J15" t="s">
-        <v>62</v>
+        <v>38</v>
       </c>
       <c r="K15" t="s">
-        <v>79</v>
+        <v>185</v>
       </c>
       <c r="L15" t="s">
-        <v>156</v>
+        <v>125</v>
       </c>
       <c r="N15" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="16" spans="1:15" x14ac:dyDescent="0.25">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="16" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
-        <v>81</v>
+        <v>68</v>
       </c>
       <c r="B16" t="s">
-        <v>82</v>
+        <v>69</v>
       </c>
       <c r="C16" t="s">
-        <v>83</v>
+        <v>70</v>
       </c>
       <c r="D16">
         <v>2018</v>
@@ -1656,33 +1656,33 @@
         <v>18</v>
       </c>
       <c r="G16" t="s">
-        <v>166</v>
+        <v>134</v>
       </c>
       <c r="H16" t="s">
         <v>19</v>
       </c>
       <c r="I16" t="s">
-        <v>167</v>
+        <v>135</v>
       </c>
       <c r="J16" t="s">
         <v>20</v>
       </c>
       <c r="K16" t="s">
-        <v>146</v>
+        <v>169</v>
       </c>
       <c r="L16" t="s">
-        <v>157</v>
-      </c>
-    </row>
-    <row r="17" spans="1:13" x14ac:dyDescent="0.25">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="17" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="B17" t="s">
-        <v>59</v>
+        <v>51</v>
       </c>
       <c r="C17" t="s">
-        <v>56</v>
+        <v>49</v>
       </c>
       <c r="D17">
         <v>2018</v>
@@ -1691,36 +1691,36 @@
         <v>30104278</v>
       </c>
       <c r="F17" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="G17" t="s">
-        <v>178</v>
+        <v>144</v>
       </c>
       <c r="H17" t="s">
-        <v>84</v>
+        <v>71</v>
       </c>
       <c r="I17" t="s">
-        <v>167</v>
+        <v>135</v>
       </c>
       <c r="J17" t="s">
         <v>20</v>
       </c>
       <c r="K17" t="s">
-        <v>85</v>
+        <v>205</v>
       </c>
       <c r="L17" t="s">
-        <v>158</v>
-      </c>
-    </row>
-    <row r="18" spans="1:13" x14ac:dyDescent="0.25">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="18" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
-        <v>86</v>
+        <v>179</v>
       </c>
       <c r="B18" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="C18" t="s">
-        <v>74</v>
+        <v>63</v>
       </c>
       <c r="D18">
         <v>2018</v>
@@ -1729,36 +1729,36 @@
         <v>29632010</v>
       </c>
       <c r="F18" t="s">
-        <v>87</v>
+        <v>72</v>
       </c>
       <c r="G18" t="s">
-        <v>178</v>
+        <v>144</v>
       </c>
       <c r="H18" t="s">
-        <v>84</v>
+        <v>71</v>
       </c>
       <c r="I18" t="s">
-        <v>167</v>
+        <v>135</v>
       </c>
       <c r="J18" t="s">
         <v>20</v>
       </c>
       <c r="K18" t="s">
-        <v>88</v>
+        <v>206</v>
       </c>
       <c r="L18" t="s">
-        <v>159</v>
-      </c>
-    </row>
-    <row r="19" spans="1:13" x14ac:dyDescent="0.25">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="19" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
-        <v>89</v>
+        <v>73</v>
       </c>
       <c r="B19" t="s">
-        <v>82</v>
+        <v>69</v>
       </c>
       <c r="C19" t="s">
-        <v>90</v>
+        <v>74</v>
       </c>
       <c r="D19">
         <v>2018</v>
@@ -1767,36 +1767,36 @@
         <v>29463528</v>
       </c>
       <c r="F19" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="G19" t="s">
-        <v>178</v>
+        <v>144</v>
       </c>
       <c r="H19" t="s">
-        <v>84</v>
+        <v>71</v>
       </c>
       <c r="I19" t="s">
-        <v>179</v>
+        <v>145</v>
       </c>
       <c r="J19" t="s">
         <v>20</v>
       </c>
       <c r="K19" t="s">
-        <v>91</v>
+        <v>207</v>
       </c>
       <c r="L19" t="s">
-        <v>160</v>
-      </c>
-    </row>
-    <row r="20" spans="1:13" x14ac:dyDescent="0.25">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="20" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
-        <v>92</v>
+        <v>75</v>
       </c>
       <c r="B20" t="s">
-        <v>93</v>
+        <v>76</v>
       </c>
       <c r="C20" t="s">
-        <v>94</v>
+        <v>77</v>
       </c>
       <c r="D20">
         <v>2018</v>
@@ -1805,36 +1805,36 @@
         <v>29437610</v>
       </c>
       <c r="F20" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="G20" t="s">
-        <v>178</v>
+        <v>144</v>
       </c>
       <c r="H20" t="s">
-        <v>84</v>
+        <v>71</v>
       </c>
       <c r="I20" t="s">
-        <v>167</v>
+        <v>135</v>
       </c>
       <c r="J20" t="s">
         <v>20</v>
       </c>
       <c r="K20" t="s">
-        <v>95</v>
+        <v>208</v>
       </c>
       <c r="L20" t="s">
-        <v>158</v>
-      </c>
-    </row>
-    <row r="21" spans="1:13" x14ac:dyDescent="0.25">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="21" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
-        <v>49</v>
+        <v>43</v>
       </c>
       <c r="B21" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="C21" t="s">
-        <v>96</v>
+        <v>78</v>
       </c>
       <c r="D21">
         <v>2018</v>
@@ -1846,33 +1846,33 @@
         <v>24</v>
       </c>
       <c r="G21" t="s">
-        <v>176</v>
+        <v>142</v>
       </c>
       <c r="H21" t="s">
         <v>19</v>
       </c>
       <c r="I21" t="s">
-        <v>180</v>
+        <v>146</v>
       </c>
       <c r="J21" t="s">
         <v>20</v>
       </c>
       <c r="K21" t="s">
-        <v>199</v>
+        <v>186</v>
       </c>
       <c r="L21" t="s">
-        <v>196</v>
-      </c>
-    </row>
-    <row r="22" spans="1:13" x14ac:dyDescent="0.25">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="22" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
-        <v>97</v>
+        <v>79</v>
       </c>
       <c r="B22" t="s">
-        <v>44</v>
+        <v>39</v>
       </c>
       <c r="C22" t="s">
-        <v>94</v>
+        <v>77</v>
       </c>
       <c r="D22">
         <v>2018</v>
@@ -1884,33 +1884,33 @@
         <v>18</v>
       </c>
       <c r="G22" t="s">
-        <v>178</v>
+        <v>136</v>
       </c>
       <c r="H22" t="s">
-        <v>84</v>
+        <v>194</v>
       </c>
       <c r="I22" t="s">
-        <v>181</v>
+        <v>147</v>
       </c>
       <c r="J22" t="s">
         <v>20</v>
       </c>
       <c r="K22" t="s">
-        <v>98</v>
+        <v>195</v>
       </c>
       <c r="L22" t="s">
-        <v>161</v>
-      </c>
-    </row>
-    <row r="23" spans="1:13" x14ac:dyDescent="0.25">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="23" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
-        <v>97</v>
+        <v>79</v>
       </c>
       <c r="B23" t="s">
-        <v>82</v>
+        <v>69</v>
       </c>
       <c r="C23" t="s">
-        <v>90</v>
+        <v>74</v>
       </c>
       <c r="D23">
         <v>2017</v>
@@ -1919,39 +1919,39 @@
         <v>28993331</v>
       </c>
       <c r="F23" t="s">
-        <v>182</v>
+        <v>148</v>
       </c>
       <c r="G23" t="s">
-        <v>168</v>
+        <v>136</v>
       </c>
       <c r="H23" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="I23" t="s">
-        <v>183</v>
+        <v>190</v>
       </c>
       <c r="J23" t="s">
         <v>20</v>
       </c>
       <c r="K23" t="s">
-        <v>99</v>
+        <v>209</v>
       </c>
       <c r="L23" t="s">
-        <v>152</v>
+        <v>168</v>
       </c>
       <c r="M23" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="24" spans="1:13" x14ac:dyDescent="0.25">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="24" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
-        <v>101</v>
+        <v>81</v>
       </c>
       <c r="B24" t="s">
-        <v>82</v>
+        <v>69</v>
       </c>
       <c r="C24" t="s">
-        <v>90</v>
+        <v>74</v>
       </c>
       <c r="D24">
         <v>2017</v>
@@ -1963,33 +1963,33 @@
         <v>24</v>
       </c>
       <c r="G24" t="s">
-        <v>168</v>
+        <v>136</v>
       </c>
       <c r="H24" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="I24" t="s">
-        <v>173</v>
+        <v>140</v>
       </c>
       <c r="J24" t="s">
         <v>20</v>
       </c>
       <c r="K24" t="s">
-        <v>99</v>
+        <v>209</v>
       </c>
       <c r="L24" t="s">
-        <v>152</v>
-      </c>
-    </row>
-    <row r="25" spans="1:13" x14ac:dyDescent="0.25">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="25" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
-        <v>102</v>
+        <v>82</v>
       </c>
       <c r="B25" t="s">
-        <v>103</v>
+        <v>83</v>
       </c>
       <c r="C25" t="s">
-        <v>104</v>
+        <v>84</v>
       </c>
       <c r="D25">
         <v>2017</v>
@@ -2001,33 +2001,33 @@
         <v>24</v>
       </c>
       <c r="G25" t="s">
-        <v>184</v>
+        <v>149</v>
       </c>
       <c r="H25" t="s">
-        <v>105</v>
+        <v>85</v>
       </c>
       <c r="I25" t="s">
-        <v>106</v>
+        <v>192</v>
       </c>
       <c r="J25" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
       <c r="K25" t="s">
-        <v>148</v>
+        <v>118</v>
       </c>
       <c r="L25" t="s">
-        <v>162</v>
-      </c>
-    </row>
-    <row r="26" spans="1:13" x14ac:dyDescent="0.25">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="26" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
-        <v>64</v>
+        <v>54</v>
       </c>
       <c r="B26" t="s">
-        <v>107</v>
+        <v>86</v>
       </c>
       <c r="C26" t="s">
-        <v>96</v>
+        <v>78</v>
       </c>
       <c r="D26">
         <v>2017</v>
@@ -2039,33 +2039,33 @@
         <v>24</v>
       </c>
       <c r="G26" t="s">
-        <v>169</v>
+        <v>137</v>
       </c>
       <c r="H26" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
       <c r="I26" t="s">
-        <v>185</v>
+        <v>150</v>
       </c>
       <c r="J26" t="s">
-        <v>144</v>
+        <v>115</v>
       </c>
       <c r="K26" t="s">
-        <v>200</v>
+        <v>193</v>
       </c>
       <c r="L26" t="s">
-        <v>152</v>
-      </c>
-    </row>
-    <row r="27" spans="1:13" x14ac:dyDescent="0.25">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="27" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
-        <v>108</v>
+        <v>87</v>
       </c>
       <c r="B27" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="C27" t="s">
-        <v>90</v>
+        <v>74</v>
       </c>
       <c r="D27">
         <v>2016</v>
@@ -2077,33 +2077,33 @@
         <v>24</v>
       </c>
       <c r="G27" t="s">
+        <v>136</v>
+      </c>
+      <c r="H27" t="s">
+        <v>31</v>
+      </c>
+      <c r="I27" t="s">
+        <v>135</v>
+      </c>
+      <c r="J27" t="s">
+        <v>88</v>
+      </c>
+      <c r="K27" t="s">
+        <v>187</v>
+      </c>
+      <c r="L27" t="s">
         <v>168</v>
       </c>
-      <c r="H27" t="s">
-        <v>33</v>
-      </c>
-      <c r="I27" t="s">
-        <v>167</v>
-      </c>
-      <c r="J27" t="s">
-        <v>109</v>
-      </c>
-      <c r="K27" t="s">
-        <v>110</v>
-      </c>
-      <c r="L27" t="s">
-        <v>152</v>
-      </c>
-    </row>
-    <row r="28" spans="1:13" x14ac:dyDescent="0.25">
+    </row>
+    <row r="28" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
-        <v>111</v>
+        <v>171</v>
       </c>
       <c r="B28" t="s">
         <v>22</v>
       </c>
       <c r="C28" t="s">
-        <v>112</v>
+        <v>89</v>
       </c>
       <c r="D28">
         <v>2016</v>
@@ -2112,39 +2112,39 @@
         <v>27494922</v>
       </c>
       <c r="F28" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="G28" t="s">
-        <v>168</v>
+        <v>136</v>
       </c>
       <c r="H28" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="I28" t="s">
-        <v>186</v>
+        <v>180</v>
       </c>
       <c r="J28" t="s">
         <v>20</v>
       </c>
       <c r="K28" t="s">
-        <v>147</v>
+        <v>117</v>
       </c>
       <c r="L28" t="s">
-        <v>161</v>
+        <v>130</v>
       </c>
       <c r="M28" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="29" spans="1:13" x14ac:dyDescent="0.25">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="29" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
-        <v>67</v>
+        <v>57</v>
       </c>
       <c r="B29" t="s">
-        <v>93</v>
+        <v>76</v>
       </c>
       <c r="C29" t="s">
-        <v>114</v>
+        <v>91</v>
       </c>
       <c r="D29">
         <v>2016</v>
@@ -2156,33 +2156,33 @@
         <v>24</v>
       </c>
       <c r="G29" t="s">
-        <v>169</v>
+        <v>137</v>
       </c>
       <c r="H29" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
       <c r="I29" t="s">
-        <v>187</v>
+        <v>151</v>
       </c>
       <c r="J29" t="s">
-        <v>115</v>
+        <v>92</v>
       </c>
       <c r="K29" t="s">
-        <v>71</v>
+        <v>61</v>
       </c>
       <c r="L29" t="s">
-        <v>163</v>
-      </c>
-    </row>
-    <row r="30" spans="1:13" x14ac:dyDescent="0.25">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="30" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
-        <v>81</v>
+        <v>68</v>
       </c>
       <c r="B30" t="s">
-        <v>116</v>
+        <v>93</v>
       </c>
       <c r="C30" t="s">
-        <v>117</v>
+        <v>94</v>
       </c>
       <c r="D30">
         <v>2015</v>
@@ -2194,33 +2194,33 @@
         <v>18</v>
       </c>
       <c r="G30" t="s">
-        <v>166</v>
+        <v>134</v>
       </c>
       <c r="H30" t="s">
         <v>19</v>
       </c>
       <c r="I30" t="s">
-        <v>167</v>
+        <v>135</v>
       </c>
       <c r="J30" t="s">
         <v>20</v>
       </c>
       <c r="K30" t="s">
-        <v>146</v>
+        <v>169</v>
       </c>
       <c r="L30" t="s">
-        <v>164</v>
-      </c>
-    </row>
-    <row r="31" spans="1:13" x14ac:dyDescent="0.25">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="31" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
-        <v>118</v>
+        <v>95</v>
       </c>
       <c r="B31" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="C31" t="s">
-        <v>119</v>
+        <v>96</v>
       </c>
       <c r="D31">
         <v>2015</v>
@@ -2232,36 +2232,36 @@
         <v>18</v>
       </c>
       <c r="G31" t="s">
-        <v>168</v>
+        <v>136</v>
       </c>
       <c r="H31" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="I31" t="s">
-        <v>188</v>
+        <v>152</v>
       </c>
       <c r="J31" t="s">
         <v>20</v>
       </c>
       <c r="K31" t="s">
-        <v>120</v>
+        <v>188</v>
       </c>
       <c r="L31" t="s">
-        <v>161</v>
+        <v>130</v>
       </c>
       <c r="M31" t="s">
-        <v>121</v>
-      </c>
-    </row>
-    <row r="32" spans="1:13" x14ac:dyDescent="0.25">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="32" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
-        <v>122</v>
+        <v>98</v>
       </c>
       <c r="B32" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C32" t="s">
-        <v>90</v>
+        <v>74</v>
       </c>
       <c r="D32">
         <v>2015</v>
@@ -2273,33 +2273,33 @@
         <v>24</v>
       </c>
       <c r="G32" t="s">
-        <v>168</v>
+        <v>136</v>
       </c>
       <c r="H32" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="I32" t="s">
-        <v>167</v>
+        <v>135</v>
       </c>
       <c r="J32" t="s">
-        <v>109</v>
+        <v>88</v>
       </c>
       <c r="K32" t="s">
-        <v>147</v>
+        <v>117</v>
       </c>
       <c r="L32" t="s">
-        <v>163</v>
-      </c>
-    </row>
-    <row r="33" spans="1:14" x14ac:dyDescent="0.25">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="33" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
-        <v>123</v>
+        <v>99</v>
       </c>
       <c r="B33" t="s">
-        <v>124</v>
+        <v>100</v>
       </c>
       <c r="C33" t="s">
-        <v>125</v>
+        <v>101</v>
       </c>
       <c r="D33">
         <v>2015</v>
@@ -2308,36 +2308,36 @@
         <v>25465523</v>
       </c>
       <c r="F33" t="s">
-        <v>70</v>
+        <v>60</v>
       </c>
       <c r="G33" t="s">
+        <v>137</v>
+      </c>
+      <c r="H33" t="s">
+        <v>37</v>
+      </c>
+      <c r="I33" t="s">
+        <v>135</v>
+      </c>
+      <c r="J33" t="s">
+        <v>38</v>
+      </c>
+      <c r="K33" t="s">
         <v>169</v>
       </c>
-      <c r="H33" t="s">
-        <v>41</v>
-      </c>
-      <c r="I33" t="s">
-        <v>167</v>
-      </c>
-      <c r="J33" t="s">
-        <v>62</v>
-      </c>
-      <c r="K33" t="s">
-        <v>146</v>
-      </c>
       <c r="L33" t="s">
-        <v>165</v>
-      </c>
-    </row>
-    <row r="34" spans="1:14" x14ac:dyDescent="0.25">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="34" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
-        <v>126</v>
+        <v>102</v>
       </c>
       <c r="B34" t="s">
-        <v>82</v>
+        <v>69</v>
       </c>
       <c r="C34" t="s">
-        <v>127</v>
+        <v>103</v>
       </c>
       <c r="D34">
         <v>2015</v>
@@ -2346,39 +2346,39 @@
         <v>25362196</v>
       </c>
       <c r="F34" t="s">
-        <v>182</v>
+        <v>148</v>
       </c>
       <c r="G34" t="s">
-        <v>166</v>
+        <v>134</v>
       </c>
       <c r="H34" t="s">
         <v>19</v>
       </c>
       <c r="I34" t="s">
-        <v>167</v>
+        <v>135</v>
       </c>
       <c r="J34" t="s">
-        <v>145</v>
+        <v>116</v>
       </c>
       <c r="K34" t="s">
-        <v>146</v>
+        <v>169</v>
       </c>
       <c r="L34" t="s">
-        <v>152</v>
+        <v>168</v>
       </c>
       <c r="M34" t="s">
-        <v>128</v>
-      </c>
-    </row>
-    <row r="35" spans="1:14" x14ac:dyDescent="0.25">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="35" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
-        <v>129</v>
+        <v>170</v>
       </c>
       <c r="B35" t="s">
-        <v>103</v>
+        <v>83</v>
       </c>
       <c r="C35" t="s">
-        <v>94</v>
+        <v>77</v>
       </c>
       <c r="D35">
         <v>2013</v>
@@ -2390,33 +2390,33 @@
         <v>24</v>
       </c>
       <c r="G35" t="s">
-        <v>168</v>
+        <v>136</v>
       </c>
       <c r="H35" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="I35" t="s">
-        <v>189</v>
+        <v>153</v>
       </c>
       <c r="J35" t="s">
         <v>20</v>
       </c>
       <c r="K35" t="s">
-        <v>147</v>
+        <v>117</v>
       </c>
       <c r="L35" t="s">
-        <v>152</v>
-      </c>
-    </row>
-    <row r="36" spans="1:14" x14ac:dyDescent="0.25">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="36" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
-        <v>192</v>
+        <v>156</v>
       </c>
       <c r="B36" t="s">
-        <v>130</v>
+        <v>105</v>
       </c>
       <c r="C36" t="s">
-        <v>131</v>
+        <v>106</v>
       </c>
       <c r="D36">
         <v>2013</v>
@@ -2428,33 +2428,33 @@
         <v>24</v>
       </c>
       <c r="G36" t="s">
-        <v>190</v>
+        <v>154</v>
       </c>
       <c r="H36" t="s">
         <v>19</v>
       </c>
       <c r="I36" t="s">
-        <v>167</v>
+        <v>135</v>
       </c>
       <c r="J36" t="s">
-        <v>132</v>
+        <v>107</v>
       </c>
       <c r="K36" t="s">
-        <v>195</v>
+        <v>157</v>
       </c>
       <c r="L36" t="s">
-        <v>152</v>
-      </c>
-    </row>
-    <row r="37" spans="1:14" x14ac:dyDescent="0.25">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="37" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
-        <v>111</v>
+        <v>171</v>
       </c>
       <c r="B37" t="s">
-        <v>133</v>
+        <v>108</v>
       </c>
       <c r="C37" t="s">
-        <v>119</v>
+        <v>96</v>
       </c>
       <c r="D37">
         <v>2016</v>
@@ -2466,36 +2466,36 @@
         <v>24</v>
       </c>
       <c r="G37" t="s">
-        <v>168</v>
+        <v>136</v>
       </c>
       <c r="H37" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="I37" t="s">
-        <v>134</v>
+        <v>181</v>
       </c>
       <c r="J37" t="s">
-        <v>135</v>
+        <v>109</v>
       </c>
       <c r="K37" t="s">
-        <v>136</v>
+        <v>172</v>
       </c>
       <c r="L37" t="s">
-        <v>163</v>
+        <v>131</v>
       </c>
       <c r="N37" t="s">
-        <v>137</v>
-      </c>
-    </row>
-    <row r="38" spans="1:14" x14ac:dyDescent="0.25">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="38" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
-        <v>138</v>
+        <v>182</v>
       </c>
       <c r="B38" t="s">
-        <v>68</v>
+        <v>58</v>
       </c>
       <c r="C38" t="s">
-        <v>139</v>
+        <v>111</v>
       </c>
       <c r="D38">
         <v>2017</v>
@@ -2504,39 +2504,39 @@
         <v>27634916</v>
       </c>
       <c r="F38" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="G38" t="s">
-        <v>191</v>
+        <v>155</v>
       </c>
       <c r="H38" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="I38" t="s">
-        <v>140</v>
+        <v>112</v>
       </c>
       <c r="J38" t="s">
-        <v>141</v>
+        <v>113</v>
       </c>
       <c r="K38" t="s">
-        <v>142</v>
+        <v>183</v>
       </c>
       <c r="L38" t="s">
+        <v>130</v>
+      </c>
+      <c r="N38" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="39" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A39" t="s">
+        <v>162</v>
+      </c>
+      <c r="B39" t="s">
+        <v>160</v>
+      </c>
+      <c r="C39" t="s">
         <v>161</v>
-      </c>
-      <c r="N38" t="s">
-        <v>143</v>
-      </c>
-    </row>
-    <row r="39" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A39" t="s">
-        <v>203</v>
-      </c>
-      <c r="B39" t="s">
-        <v>201</v>
-      </c>
-      <c r="C39" t="s">
-        <v>202</v>
       </c>
       <c r="D39">
         <v>1963</v>
@@ -2548,33 +2548,33 @@
         <v>24</v>
       </c>
       <c r="G39" t="s">
-        <v>190</v>
+        <v>154</v>
       </c>
       <c r="H39" t="s">
         <v>19</v>
       </c>
       <c r="I39" t="s">
-        <v>204</v>
+        <v>163</v>
       </c>
       <c r="J39" t="s">
-        <v>145</v>
+        <v>116</v>
       </c>
       <c r="K39" t="s">
-        <v>147</v>
+        <v>117</v>
       </c>
       <c r="L39" t="s">
-        <v>152</v>
-      </c>
-    </row>
-    <row r="40" spans="1:14" x14ac:dyDescent="0.25">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="40" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
-        <v>92</v>
+        <v>75</v>
       </c>
       <c r="B40" t="s">
-        <v>205</v>
+        <v>164</v>
       </c>
       <c r="C40" t="s">
-        <v>90</v>
+        <v>74</v>
       </c>
       <c r="D40">
         <v>2019</v>
@@ -2583,36 +2583,36 @@
         <v>31636062</v>
       </c>
       <c r="F40" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="G40" t="s">
-        <v>178</v>
+        <v>144</v>
       </c>
       <c r="H40" t="s">
-        <v>84</v>
+        <v>71</v>
       </c>
       <c r="I40" t="s">
-        <v>173</v>
+        <v>140</v>
       </c>
       <c r="J40" t="s">
         <v>20</v>
       </c>
       <c r="K40" t="s">
-        <v>147</v>
+        <v>117</v>
       </c>
       <c r="L40" t="s">
-        <v>160</v>
-      </c>
-    </row>
-    <row r="41" spans="1:14" x14ac:dyDescent="0.25">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="41" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
-        <v>138</v>
+        <v>182</v>
       </c>
       <c r="B41" t="s">
-        <v>207</v>
+        <v>166</v>
       </c>
       <c r="C41" t="s">
-        <v>206</v>
+        <v>165</v>
       </c>
       <c r="D41">
         <v>2020</v>
@@ -2624,22 +2624,22 @@
         <v>18</v>
       </c>
       <c r="G41" t="s">
-        <v>191</v>
+        <v>155</v>
       </c>
       <c r="H41" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="I41" t="s">
-        <v>208</v>
+        <v>167</v>
       </c>
       <c r="J41" t="s">
         <v>20</v>
       </c>
       <c r="K41" t="s">
-        <v>209</v>
+        <v>189</v>
       </c>
       <c r="L41" t="s">
-        <v>161</v>
+        <v>130</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Update layout and correct errors
</commit_message>
<xml_diff>
--- a/tables/combination_drugs.xlsx
+++ b/tables/combination_drugs.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="24527"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="24701"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Vincent\Documents\pmx-models-atb-review\tables\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FAD05E32-D512-4F7B-ABFF-3486228AB56E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{68DC73D1-FFE9-4079-9397-C5398C86DCA2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1464" yWindow="1464" windowWidth="17280" windowHeight="8964" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1116" yWindow="1116" windowWidth="17280" windowHeight="8964" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -157,12 +157,6 @@
     <t>Klebsiella pneumoniae, 2 strains;Escherichia coli, 1 strains;Enterobacter cloacae, 1 strains</t>
   </si>
   <si>
-    <t>Krsitoffersson</t>
-  </si>
-  <si>
-    <t>subpopulations, NA;other, beta lacatamases degrading ceftazidime</t>
-  </si>
-  <si>
     <t>ciprofloxacin + tobramycin</t>
   </si>
   <si>
@@ -385,9 +379,6 @@
     <t>critically ill, simulations</t>
   </si>
   <si>
-    <t>critically ill with arc, simulations;critically ill with arc, experimental setup</t>
-  </si>
-  <si>
     <t>cystic fibrosis patients, simulations</t>
   </si>
   <si>
@@ -445,9 +436,6 @@
     <t>Emax, death, no, NA, NA, NA</t>
   </si>
   <si>
-    <t>1 metabolic state, emax growth, no delay</t>
-  </si>
-  <si>
     <t>1 metabolic state, logistic growth, delay</t>
   </si>
   <si>
@@ -499,9 +487,6 @@
     <t>patients, experimental setup</t>
   </si>
   <si>
-    <t>linear power, death, no, NA, NA, NA</t>
-  </si>
-  <si>
     <t>Escherichia coli</t>
   </si>
   <si>
@@ -574,18 +559,9 @@
     <t>additivity, decrease in EC50, polymyxin B, meropenem, threshold of polymyxin B concentration above which EC50 of meropenem decreases</t>
   </si>
   <si>
-    <t>additivity, decrease in EC50, avibactam, aztreonam, biexponential equation of aztronam EC50 dependent on avibactam concentrations;additivity, decrease in drug degradation rate, avibactam, aztreonam, NA</t>
-  </si>
-  <si>
-    <t>additivity, decrease in EC50, fusidic acid, colistin, NA;additivity, increase in emax, colistin, fusidic acid, NA</t>
-  </si>
-  <si>
     <t>additivity, decrease in EC50, avibactam, ceftazidime, biexponential equation of ceftazidime EC50 dependent on avibactam concentrations;additivity, decrease in drug degradation rate, avibactam, ceftazidime, NA</t>
   </si>
   <si>
-    <t>additivity, decrease in EC50, tobramycin, imipenem, emax equation;additivity, decrease in EC50, amikacin, imipenem, emax equation</t>
-  </si>
-  <si>
     <t>additivity, decrease in EC50, colistin, doripenem, not a continuous relationship: different doripenem EC50 values for discrete colistin concentrations</t>
   </si>
   <si>
@@ -616,12 +592,6 @@
     <t>additivity, decrease in EC50, fosfomycin, sulbactam, GPDI like</t>
   </si>
   <si>
-    <t>additivity, decrease in EC50, polymyxin B, meroepenm, GPDI like</t>
-  </si>
-  <si>
-    <t>additivity, increase in emax, polymyxin B, minocycline, GPDI</t>
-  </si>
-  <si>
     <t>additivity, decrease in EC50, polymyxin B, minocycline, GPDI;additivity, decrease in adaptive resistance rate, minocycline, polymyxin B, GPDI</t>
   </si>
   <si>
@@ -650,6 +620,36 @@
   </si>
   <si>
     <t>additivity, decrease in EC50, tobramycin, imipenem, GPDI like</t>
+  </si>
+  <si>
+    <t>1 metabolic state, Emax growth, no delay</t>
+  </si>
+  <si>
+    <t>additivity, decrease in EC50, avibactam, aztreonam, biexponential equation of aztreonam EC50 dependent on avibactam concentrations;additivity, decrease in drug degradation rate, avibactam, aztreonam, NA</t>
+  </si>
+  <si>
+    <t>Kristoffersson</t>
+  </si>
+  <si>
+    <t>subpopulations, NA;other, beta-lactamases degrading ceftazidime</t>
+  </si>
+  <si>
+    <t>linear-power, death, no, NA, NA, NA</t>
+  </si>
+  <si>
+    <t>additivity, increase in Emax, polymyxin B, minocycline, GPDI</t>
+  </si>
+  <si>
+    <t>additivity, decrease in EC50, fusidic acid, colistin, NA;additivity, increase in Emax, colistin, fusidic acid, NA</t>
+  </si>
+  <si>
+    <t>additivity, decrease in EC50, tobramycin, imipenem, Emax equation;additivity, decrease in EC50, amikacin, imipenem, Emax equation</t>
+  </si>
+  <si>
+    <t>additivity, decrease in EC50, polymyxin B, meropenem, GPDI like</t>
+  </si>
+  <si>
+    <t>critically ill with ARC, simulations;critically ill with arc, experimental setup</t>
   </si>
 </sst>
 </file>
@@ -1039,8 +1039,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:O41"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C7" workbookViewId="0">
-      <selection activeCell="L16" sqref="L16"/>
+    <sheetView tabSelected="1" topLeftCell="G1" workbookViewId="0">
+      <selection activeCell="N21" sqref="N21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1112,22 +1112,22 @@
         <v>18</v>
       </c>
       <c r="G2" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="H2" t="s">
         <v>19</v>
       </c>
       <c r="I2" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
       <c r="J2" t="s">
         <v>20</v>
       </c>
       <c r="K2" t="s">
-        <v>169</v>
+        <v>164</v>
       </c>
       <c r="L2" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
     </row>
     <row r="3" spans="1:15" x14ac:dyDescent="0.3">
@@ -1150,22 +1150,22 @@
         <v>24</v>
       </c>
       <c r="G3" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="H3" t="s">
         <v>19</v>
       </c>
       <c r="I3" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
       <c r="J3" t="s">
         <v>20</v>
       </c>
       <c r="K3" t="s">
-        <v>196</v>
+        <v>188</v>
       </c>
       <c r="L3" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
     </row>
     <row r="4" spans="1:15" x14ac:dyDescent="0.3">
@@ -1188,22 +1188,22 @@
         <v>24</v>
       </c>
       <c r="G4" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="H4" t="s">
         <v>19</v>
       </c>
       <c r="I4" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
       <c r="J4" t="s">
         <v>20</v>
       </c>
       <c r="K4" t="s">
-        <v>197</v>
+        <v>189</v>
       </c>
       <c r="L4" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
     </row>
     <row r="5" spans="1:15" x14ac:dyDescent="0.3">
@@ -1226,7 +1226,7 @@
         <v>30</v>
       </c>
       <c r="G5" t="s">
-        <v>136</v>
+        <v>133</v>
       </c>
       <c r="H5" t="s">
         <v>31</v>
@@ -1238,15 +1238,15 @@
         <v>20</v>
       </c>
       <c r="K5" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="L5" t="s">
-        <v>121</v>
+        <v>209</v>
       </c>
     </row>
     <row r="6" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>173</v>
+        <v>168</v>
       </c>
       <c r="B6" t="s">
         <v>33</v>
@@ -1264,22 +1264,22 @@
         <v>18</v>
       </c>
       <c r="G6" t="s">
-        <v>136</v>
+        <v>133</v>
       </c>
       <c r="H6" t="s">
         <v>31</v>
       </c>
       <c r="I6" t="s">
-        <v>174</v>
+        <v>169</v>
       </c>
       <c r="J6" t="s">
         <v>20</v>
       </c>
       <c r="K6" t="s">
-        <v>198</v>
+        <v>208</v>
       </c>
       <c r="L6" t="s">
-        <v>168</v>
+        <v>163</v>
       </c>
       <c r="M6" t="s">
         <v>35</v>
@@ -1287,7 +1287,7 @@
     </row>
     <row r="7" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>175</v>
+        <v>170</v>
       </c>
       <c r="B7" t="s">
         <v>33</v>
@@ -1305,30 +1305,30 @@
         <v>24</v>
       </c>
       <c r="G7" t="s">
-        <v>137</v>
+        <v>134</v>
       </c>
       <c r="H7" t="s">
         <v>37</v>
       </c>
       <c r="I7" t="s">
-        <v>159</v>
+        <v>204</v>
       </c>
       <c r="J7" t="s">
         <v>38</v>
       </c>
       <c r="K7" t="s">
-        <v>199</v>
+        <v>205</v>
       </c>
       <c r="L7" t="s">
-        <v>168</v>
+        <v>163</v>
       </c>
       <c r="M7" t="s">
-        <v>138</v>
+        <v>135</v>
       </c>
     </row>
     <row r="8" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>175</v>
+        <v>170</v>
       </c>
       <c r="B8" t="s">
         <v>39</v>
@@ -1346,22 +1346,22 @@
         <v>24</v>
       </c>
       <c r="G8" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="H8" t="s">
         <v>19</v>
       </c>
       <c r="I8" t="s">
-        <v>176</v>
+        <v>171</v>
       </c>
       <c r="J8" t="s">
         <v>41</v>
       </c>
       <c r="K8" t="s">
-        <v>200</v>
+        <v>190</v>
       </c>
       <c r="L8" t="s">
-        <v>168</v>
+        <v>163</v>
       </c>
       <c r="N8" t="s">
         <v>42</v>
@@ -1375,7 +1375,7 @@
         <v>44</v>
       </c>
       <c r="C9" t="s">
-        <v>45</v>
+        <v>202</v>
       </c>
       <c r="D9">
         <v>2020</v>
@@ -1387,33 +1387,33 @@
         <v>24</v>
       </c>
       <c r="G9" t="s">
-        <v>137</v>
+        <v>134</v>
       </c>
       <c r="H9" t="s">
         <v>37</v>
       </c>
       <c r="I9" t="s">
-        <v>139</v>
+        <v>136</v>
       </c>
       <c r="J9" t="s">
-        <v>46</v>
+        <v>203</v>
       </c>
       <c r="K9" t="s">
-        <v>201</v>
+        <v>191</v>
       </c>
       <c r="L9" t="s">
-        <v>122</v>
+        <v>119</v>
       </c>
     </row>
     <row r="10" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
+        <v>45</v>
+      </c>
+      <c r="B10" t="s">
+        <v>46</v>
+      </c>
+      <c r="C10" t="s">
         <v>47</v>
-      </c>
-      <c r="B10" t="s">
-        <v>48</v>
-      </c>
-      <c r="C10" t="s">
-        <v>49</v>
       </c>
       <c r="D10">
         <v>2019</v>
@@ -1425,33 +1425,33 @@
         <v>24</v>
       </c>
       <c r="G10" t="s">
-        <v>136</v>
+        <v>133</v>
       </c>
       <c r="H10" t="s">
         <v>31</v>
       </c>
       <c r="I10" t="s">
-        <v>140</v>
+        <v>137</v>
       </c>
       <c r="J10" t="s">
         <v>20</v>
       </c>
       <c r="K10" t="s">
-        <v>202</v>
+        <v>192</v>
       </c>
       <c r="L10" t="s">
-        <v>168</v>
+        <v>163</v>
       </c>
     </row>
     <row r="11" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
+        <v>48</v>
+      </c>
+      <c r="B11" t="s">
+        <v>49</v>
+      </c>
+      <c r="C11" t="s">
         <v>50</v>
-      </c>
-      <c r="B11" t="s">
-        <v>51</v>
-      </c>
-      <c r="C11" t="s">
-        <v>52</v>
       </c>
       <c r="D11">
         <v>2019</v>
@@ -1460,36 +1460,36 @@
         <v>31479762</v>
       </c>
       <c r="F11" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="G11" t="s">
-        <v>137</v>
+        <v>134</v>
       </c>
       <c r="H11" t="s">
         <v>37</v>
       </c>
       <c r="I11" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
       <c r="J11" t="s">
         <v>38</v>
       </c>
       <c r="K11" t="s">
-        <v>203</v>
+        <v>193</v>
       </c>
       <c r="L11" t="s">
-        <v>123</v>
+        <v>120</v>
       </c>
     </row>
     <row r="12" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
+        <v>52</v>
+      </c>
+      <c r="B12" t="s">
+        <v>53</v>
+      </c>
+      <c r="C12" t="s">
         <v>54</v>
-      </c>
-      <c r="B12" t="s">
-        <v>55</v>
-      </c>
-      <c r="C12" t="s">
-        <v>56</v>
       </c>
       <c r="D12">
         <v>2019</v>
@@ -1501,33 +1501,33 @@
         <v>24</v>
       </c>
       <c r="G12" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="H12" t="s">
         <v>19</v>
       </c>
       <c r="I12" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
       <c r="J12" t="s">
         <v>20</v>
       </c>
       <c r="K12" t="s">
-        <v>184</v>
+        <v>201</v>
       </c>
       <c r="L12" t="s">
-        <v>124</v>
+        <v>121</v>
       </c>
     </row>
     <row r="13" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
+        <v>55</v>
+      </c>
+      <c r="B13" t="s">
+        <v>56</v>
+      </c>
+      <c r="C13" t="s">
         <v>57</v>
-      </c>
-      <c r="B13" t="s">
-        <v>58</v>
-      </c>
-      <c r="C13" t="s">
-        <v>59</v>
       </c>
       <c r="D13">
         <v>2019</v>
@@ -1536,36 +1536,36 @@
         <v>30745385</v>
       </c>
       <c r="F13" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="G13" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="H13" t="s">
         <v>19</v>
       </c>
       <c r="I13" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
       <c r="J13" t="s">
         <v>38</v>
       </c>
       <c r="K13" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="L13" t="s">
-        <v>123</v>
+        <v>120</v>
       </c>
     </row>
     <row r="14" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>177</v>
+        <v>172</v>
       </c>
       <c r="B14" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="C14" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="D14">
         <v>2019</v>
@@ -1577,33 +1577,33 @@
         <v>24</v>
       </c>
       <c r="G14" t="s">
-        <v>141</v>
+        <v>200</v>
       </c>
       <c r="H14" t="s">
         <v>19</v>
       </c>
       <c r="I14" t="s">
-        <v>178</v>
+        <v>173</v>
       </c>
       <c r="J14" t="s">
         <v>20</v>
       </c>
       <c r="K14" t="s">
-        <v>204</v>
+        <v>194</v>
       </c>
       <c r="L14" t="s">
-        <v>168</v>
+        <v>163</v>
       </c>
     </row>
     <row r="15" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
+        <v>62</v>
+      </c>
+      <c r="B15" t="s">
+        <v>63</v>
+      </c>
+      <c r="C15" t="s">
         <v>64</v>
-      </c>
-      <c r="B15" t="s">
-        <v>65</v>
-      </c>
-      <c r="C15" t="s">
-        <v>66</v>
       </c>
       <c r="D15">
         <v>2019</v>
@@ -1615,36 +1615,36 @@
         <v>24</v>
       </c>
       <c r="G15" t="s">
-        <v>142</v>
+        <v>138</v>
       </c>
       <c r="H15" t="s">
         <v>19</v>
       </c>
       <c r="I15" t="s">
-        <v>143</v>
+        <v>139</v>
       </c>
       <c r="J15" t="s">
         <v>38</v>
       </c>
       <c r="K15" t="s">
-        <v>185</v>
+        <v>206</v>
       </c>
       <c r="L15" t="s">
-        <v>125</v>
+        <v>122</v>
       </c>
       <c r="N15" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
     </row>
     <row r="16" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
+        <v>66</v>
+      </c>
+      <c r="B16" t="s">
+        <v>67</v>
+      </c>
+      <c r="C16" t="s">
         <v>68</v>
-      </c>
-      <c r="B16" t="s">
-        <v>69</v>
-      </c>
-      <c r="C16" t="s">
-        <v>70</v>
       </c>
       <c r="D16">
         <v>2018</v>
@@ -1656,22 +1656,22 @@
         <v>18</v>
       </c>
       <c r="G16" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="H16" t="s">
         <v>19</v>
       </c>
       <c r="I16" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
       <c r="J16" t="s">
         <v>20</v>
       </c>
       <c r="K16" t="s">
-        <v>169</v>
+        <v>164</v>
       </c>
       <c r="L16" t="s">
-        <v>126</v>
+        <v>123</v>
       </c>
     </row>
     <row r="17" spans="1:13" x14ac:dyDescent="0.3">
@@ -1679,10 +1679,10 @@
         <v>27</v>
       </c>
       <c r="B17" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="C17" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="D17">
         <v>2018</v>
@@ -1694,33 +1694,33 @@
         <v>30</v>
       </c>
       <c r="G17" t="s">
-        <v>144</v>
+        <v>140</v>
       </c>
       <c r="H17" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="I17" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
       <c r="J17" t="s">
         <v>20</v>
       </c>
       <c r="K17" t="s">
-        <v>205</v>
+        <v>195</v>
       </c>
       <c r="L17" t="s">
-        <v>127</v>
+        <v>124</v>
       </c>
     </row>
     <row r="18" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
-        <v>179</v>
+        <v>174</v>
       </c>
       <c r="B18" t="s">
         <v>28</v>
       </c>
       <c r="C18" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="D18">
         <v>2018</v>
@@ -1729,36 +1729,36 @@
         <v>29632010</v>
       </c>
       <c r="F18" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="G18" t="s">
-        <v>144</v>
+        <v>140</v>
       </c>
       <c r="H18" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="I18" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
       <c r="J18" t="s">
         <v>20</v>
       </c>
       <c r="K18" t="s">
-        <v>206</v>
+        <v>196</v>
       </c>
       <c r="L18" t="s">
-        <v>128</v>
+        <v>125</v>
       </c>
     </row>
     <row r="19" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="B19" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="C19" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="D19">
         <v>2018</v>
@@ -1770,33 +1770,33 @@
         <v>30</v>
       </c>
       <c r="G19" t="s">
-        <v>144</v>
+        <v>140</v>
       </c>
       <c r="H19" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="I19" t="s">
-        <v>145</v>
+        <v>141</v>
       </c>
       <c r="J19" t="s">
         <v>20</v>
       </c>
       <c r="K19" t="s">
-        <v>207</v>
+        <v>197</v>
       </c>
       <c r="L19" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
     </row>
     <row r="20" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
+        <v>73</v>
+      </c>
+      <c r="B20" t="s">
+        <v>74</v>
+      </c>
+      <c r="C20" t="s">
         <v>75</v>
-      </c>
-      <c r="B20" t="s">
-        <v>76</v>
-      </c>
-      <c r="C20" t="s">
-        <v>77</v>
       </c>
       <c r="D20">
         <v>2018</v>
@@ -1808,22 +1808,22 @@
         <v>30</v>
       </c>
       <c r="G20" t="s">
-        <v>144</v>
+        <v>140</v>
       </c>
       <c r="H20" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="I20" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
       <c r="J20" t="s">
         <v>20</v>
       </c>
       <c r="K20" t="s">
-        <v>208</v>
+        <v>198</v>
       </c>
       <c r="L20" t="s">
-        <v>127</v>
+        <v>124</v>
       </c>
     </row>
     <row r="21" spans="1:13" x14ac:dyDescent="0.3">
@@ -1834,7 +1834,7 @@
         <v>28</v>
       </c>
       <c r="C21" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="D21">
         <v>2018</v>
@@ -1846,33 +1846,33 @@
         <v>24</v>
       </c>
       <c r="G21" t="s">
-        <v>142</v>
+        <v>138</v>
       </c>
       <c r="H21" t="s">
         <v>19</v>
       </c>
       <c r="I21" t="s">
-        <v>146</v>
+        <v>142</v>
       </c>
       <c r="J21" t="s">
         <v>20</v>
       </c>
       <c r="K21" t="s">
-        <v>186</v>
+        <v>179</v>
       </c>
       <c r="L21" t="s">
-        <v>158</v>
+        <v>154</v>
       </c>
     </row>
     <row r="22" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="B22" t="s">
         <v>39</v>
       </c>
       <c r="C22" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="D22">
         <v>2018</v>
@@ -1884,33 +1884,33 @@
         <v>18</v>
       </c>
       <c r="G22" t="s">
-        <v>136</v>
+        <v>133</v>
       </c>
       <c r="H22" t="s">
-        <v>194</v>
+        <v>186</v>
       </c>
       <c r="I22" t="s">
-        <v>147</v>
+        <v>143</v>
       </c>
       <c r="J22" t="s">
         <v>20</v>
       </c>
       <c r="K22" t="s">
-        <v>195</v>
+        <v>187</v>
       </c>
       <c r="L22" t="s">
-        <v>130</v>
+        <v>127</v>
       </c>
     </row>
     <row r="23" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="B23" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="C23" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="D23">
         <v>2017</v>
@@ -1919,39 +1919,39 @@
         <v>28993331</v>
       </c>
       <c r="F23" t="s">
-        <v>148</v>
+        <v>144</v>
       </c>
       <c r="G23" t="s">
-        <v>136</v>
+        <v>133</v>
       </c>
       <c r="H23" t="s">
         <v>31</v>
       </c>
       <c r="I23" t="s">
-        <v>190</v>
+        <v>182</v>
       </c>
       <c r="J23" t="s">
         <v>20</v>
       </c>
       <c r="K23" t="s">
-        <v>209</v>
+        <v>199</v>
       </c>
       <c r="L23" t="s">
-        <v>168</v>
+        <v>163</v>
       </c>
       <c r="M23" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
     </row>
     <row r="24" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="B24" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="C24" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="D24">
         <v>2017</v>
@@ -1963,33 +1963,33 @@
         <v>24</v>
       </c>
       <c r="G24" t="s">
-        <v>136</v>
+        <v>133</v>
       </c>
       <c r="H24" t="s">
         <v>31</v>
       </c>
       <c r="I24" t="s">
-        <v>140</v>
+        <v>137</v>
       </c>
       <c r="J24" t="s">
         <v>20</v>
       </c>
       <c r="K24" t="s">
-        <v>209</v>
+        <v>199</v>
       </c>
       <c r="L24" t="s">
-        <v>168</v>
+        <v>163</v>
       </c>
     </row>
     <row r="25" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
+        <v>80</v>
+      </c>
+      <c r="B25" t="s">
+        <v>81</v>
+      </c>
+      <c r="C25" t="s">
         <v>82</v>
-      </c>
-      <c r="B25" t="s">
-        <v>83</v>
-      </c>
-      <c r="C25" t="s">
-        <v>84</v>
       </c>
       <c r="D25">
         <v>2017</v>
@@ -2001,33 +2001,33 @@
         <v>24</v>
       </c>
       <c r="G25" t="s">
-        <v>149</v>
+        <v>145</v>
       </c>
       <c r="H25" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="I25" t="s">
-        <v>192</v>
+        <v>184</v>
       </c>
       <c r="J25" t="s">
         <v>38</v>
       </c>
       <c r="K25" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="L25" t="s">
-        <v>191</v>
+        <v>183</v>
       </c>
     </row>
     <row r="26" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="B26" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="C26" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="D26">
         <v>2017</v>
@@ -2039,33 +2039,33 @@
         <v>24</v>
       </c>
       <c r="G26" t="s">
-        <v>137</v>
+        <v>134</v>
       </c>
       <c r="H26" t="s">
         <v>37</v>
       </c>
       <c r="I26" t="s">
-        <v>150</v>
+        <v>146</v>
       </c>
       <c r="J26" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="K26" t="s">
-        <v>193</v>
+        <v>185</v>
       </c>
       <c r="L26" t="s">
-        <v>168</v>
+        <v>163</v>
       </c>
     </row>
     <row r="27" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="B27" t="s">
         <v>28</v>
       </c>
       <c r="C27" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="D27">
         <v>2016</v>
@@ -2077,33 +2077,33 @@
         <v>24</v>
       </c>
       <c r="G27" t="s">
-        <v>136</v>
+        <v>133</v>
       </c>
       <c r="H27" t="s">
         <v>31</v>
       </c>
       <c r="I27" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
       <c r="J27" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="K27" t="s">
-        <v>187</v>
+        <v>207</v>
       </c>
       <c r="L27" t="s">
-        <v>168</v>
+        <v>163</v>
       </c>
     </row>
     <row r="28" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
-        <v>171</v>
+        <v>166</v>
       </c>
       <c r="B28" t="s">
         <v>22</v>
       </c>
       <c r="C28" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="D28">
         <v>2016</v>
@@ -2115,36 +2115,36 @@
         <v>30</v>
       </c>
       <c r="G28" t="s">
-        <v>136</v>
+        <v>133</v>
       </c>
       <c r="H28" t="s">
         <v>31</v>
       </c>
       <c r="I28" t="s">
-        <v>180</v>
+        <v>175</v>
       </c>
       <c r="J28" t="s">
         <v>20</v>
       </c>
       <c r="K28" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="L28" t="s">
-        <v>130</v>
+        <v>127</v>
       </c>
       <c r="M28" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
     </row>
     <row r="29" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="B29" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="C29" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="D29">
         <v>2016</v>
@@ -2156,33 +2156,33 @@
         <v>24</v>
       </c>
       <c r="G29" t="s">
-        <v>137</v>
+        <v>134</v>
       </c>
       <c r="H29" t="s">
         <v>37</v>
       </c>
       <c r="I29" t="s">
-        <v>151</v>
+        <v>147</v>
       </c>
       <c r="J29" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="K29" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="L29" t="s">
-        <v>131</v>
+        <v>128</v>
       </c>
     </row>
     <row r="30" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="B30" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="C30" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="D30">
         <v>2015</v>
@@ -2194,33 +2194,33 @@
         <v>18</v>
       </c>
       <c r="G30" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="H30" t="s">
         <v>19</v>
       </c>
       <c r="I30" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
       <c r="J30" t="s">
         <v>20</v>
       </c>
       <c r="K30" t="s">
-        <v>169</v>
+        <v>164</v>
       </c>
       <c r="L30" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
     </row>
     <row r="31" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="B31" t="s">
         <v>28</v>
       </c>
       <c r="C31" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="D31">
         <v>2015</v>
@@ -2232,36 +2232,36 @@
         <v>18</v>
       </c>
       <c r="G31" t="s">
-        <v>136</v>
+        <v>133</v>
       </c>
       <c r="H31" t="s">
         <v>31</v>
       </c>
       <c r="I31" t="s">
-        <v>152</v>
+        <v>148</v>
       </c>
       <c r="J31" t="s">
         <v>20</v>
       </c>
       <c r="K31" t="s">
-        <v>188</v>
+        <v>180</v>
       </c>
       <c r="L31" t="s">
-        <v>130</v>
+        <v>127</v>
       </c>
       <c r="M31" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
     </row>
     <row r="32" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="B32" t="s">
         <v>26</v>
       </c>
       <c r="C32" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="D32">
         <v>2015</v>
@@ -2273,33 +2273,33 @@
         <v>24</v>
       </c>
       <c r="G32" t="s">
-        <v>136</v>
+        <v>133</v>
       </c>
       <c r="H32" t="s">
         <v>31</v>
       </c>
       <c r="I32" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
       <c r="J32" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="K32" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="L32" t="s">
-        <v>131</v>
+        <v>128</v>
       </c>
     </row>
     <row r="33" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
+        <v>97</v>
+      </c>
+      <c r="B33" t="s">
+        <v>98</v>
+      </c>
+      <c r="C33" t="s">
         <v>99</v>
-      </c>
-      <c r="B33" t="s">
-        <v>100</v>
-      </c>
-      <c r="C33" t="s">
-        <v>101</v>
       </c>
       <c r="D33">
         <v>2015</v>
@@ -2308,36 +2308,36 @@
         <v>25465523</v>
       </c>
       <c r="F33" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="G33" t="s">
-        <v>137</v>
+        <v>134</v>
       </c>
       <c r="H33" t="s">
         <v>37</v>
       </c>
       <c r="I33" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
       <c r="J33" t="s">
         <v>38</v>
       </c>
       <c r="K33" t="s">
-        <v>169</v>
+        <v>164</v>
       </c>
       <c r="L33" t="s">
-        <v>133</v>
+        <v>130</v>
       </c>
     </row>
     <row r="34" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="B34" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="C34" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="D34">
         <v>2015</v>
@@ -2346,39 +2346,39 @@
         <v>25362196</v>
       </c>
       <c r="F34" t="s">
-        <v>148</v>
+        <v>144</v>
       </c>
       <c r="G34" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="H34" t="s">
         <v>19</v>
       </c>
       <c r="I34" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
       <c r="J34" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="K34" t="s">
-        <v>169</v>
+        <v>164</v>
       </c>
       <c r="L34" t="s">
-        <v>168</v>
+        <v>163</v>
       </c>
       <c r="M34" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
     </row>
     <row r="35" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
-        <v>170</v>
+        <v>165</v>
       </c>
       <c r="B35" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="C35" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="D35">
         <v>2013</v>
@@ -2390,33 +2390,33 @@
         <v>24</v>
       </c>
       <c r="G35" t="s">
-        <v>136</v>
+        <v>133</v>
       </c>
       <c r="H35" t="s">
         <v>31</v>
       </c>
       <c r="I35" t="s">
-        <v>153</v>
+        <v>149</v>
       </c>
       <c r="J35" t="s">
         <v>20</v>
       </c>
       <c r="K35" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="L35" t="s">
-        <v>168</v>
+        <v>163</v>
       </c>
     </row>
     <row r="36" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
-        <v>156</v>
+        <v>152</v>
       </c>
       <c r="B36" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="C36" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="D36">
         <v>2013</v>
@@ -2428,33 +2428,33 @@
         <v>24</v>
       </c>
       <c r="G36" t="s">
-        <v>154</v>
+        <v>150</v>
       </c>
       <c r="H36" t="s">
         <v>19</v>
       </c>
       <c r="I36" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
       <c r="J36" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="K36" t="s">
-        <v>157</v>
+        <v>153</v>
       </c>
       <c r="L36" t="s">
-        <v>168</v>
+        <v>163</v>
       </c>
     </row>
     <row r="37" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
-        <v>171</v>
+        <v>166</v>
       </c>
       <c r="B37" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="C37" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="D37">
         <v>2016</v>
@@ -2466,36 +2466,36 @@
         <v>24</v>
       </c>
       <c r="G37" t="s">
-        <v>136</v>
+        <v>133</v>
       </c>
       <c r="H37" t="s">
         <v>31</v>
       </c>
       <c r="I37" t="s">
-        <v>181</v>
+        <v>176</v>
       </c>
       <c r="J37" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="K37" t="s">
-        <v>172</v>
+        <v>167</v>
       </c>
       <c r="L37" t="s">
-        <v>131</v>
+        <v>128</v>
       </c>
       <c r="N37" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
     </row>
     <row r="38" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
-        <v>182</v>
+        <v>177</v>
       </c>
       <c r="B38" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="C38" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="D38">
         <v>2017</v>
@@ -2507,36 +2507,36 @@
         <v>30</v>
       </c>
       <c r="G38" t="s">
-        <v>155</v>
+        <v>151</v>
       </c>
       <c r="H38" t="s">
         <v>31</v>
       </c>
       <c r="I38" t="s">
+        <v>110</v>
+      </c>
+      <c r="J38" t="s">
+        <v>111</v>
+      </c>
+      <c r="K38" t="s">
+        <v>178</v>
+      </c>
+      <c r="L38" t="s">
+        <v>127</v>
+      </c>
+      <c r="N38" t="s">
         <v>112</v>
-      </c>
-      <c r="J38" t="s">
-        <v>113</v>
-      </c>
-      <c r="K38" t="s">
-        <v>183</v>
-      </c>
-      <c r="L38" t="s">
-        <v>130</v>
-      </c>
-      <c r="N38" t="s">
-        <v>114</v>
       </c>
     </row>
     <row r="39" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
-        <v>162</v>
+        <v>157</v>
       </c>
       <c r="B39" t="s">
-        <v>160</v>
+        <v>155</v>
       </c>
       <c r="C39" t="s">
-        <v>161</v>
+        <v>156</v>
       </c>
       <c r="D39">
         <v>1963</v>
@@ -2548,33 +2548,33 @@
         <v>24</v>
       </c>
       <c r="G39" t="s">
-        <v>154</v>
+        <v>150</v>
       </c>
       <c r="H39" t="s">
         <v>19</v>
       </c>
       <c r="I39" t="s">
+        <v>158</v>
+      </c>
+      <c r="J39" t="s">
+        <v>114</v>
+      </c>
+      <c r="K39" t="s">
+        <v>115</v>
+      </c>
+      <c r="L39" t="s">
         <v>163</v>
-      </c>
-      <c r="J39" t="s">
-        <v>116</v>
-      </c>
-      <c r="K39" t="s">
-        <v>117</v>
-      </c>
-      <c r="L39" t="s">
-        <v>168</v>
       </c>
     </row>
     <row r="40" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="B40" t="s">
-        <v>164</v>
+        <v>159</v>
       </c>
       <c r="C40" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="D40">
         <v>2019</v>
@@ -2586,33 +2586,33 @@
         <v>30</v>
       </c>
       <c r="G40" t="s">
-        <v>144</v>
+        <v>140</v>
       </c>
       <c r="H40" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="I40" t="s">
-        <v>140</v>
+        <v>137</v>
       </c>
       <c r="J40" t="s">
         <v>20</v>
       </c>
       <c r="K40" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="L40" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
     </row>
     <row r="41" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
-        <v>182</v>
+        <v>177</v>
       </c>
       <c r="B41" t="s">
-        <v>166</v>
+        <v>161</v>
       </c>
       <c r="C41" t="s">
-        <v>165</v>
+        <v>160</v>
       </c>
       <c r="D41">
         <v>2020</v>
@@ -2624,22 +2624,22 @@
         <v>18</v>
       </c>
       <c r="G41" t="s">
-        <v>155</v>
+        <v>151</v>
       </c>
       <c r="H41" t="s">
         <v>31</v>
       </c>
       <c r="I41" t="s">
-        <v>167</v>
+        <v>162</v>
       </c>
       <c r="J41" t="s">
         <v>20</v>
       </c>
       <c r="K41" t="s">
-        <v>189</v>
+        <v>181</v>
       </c>
       <c r="L41" t="s">
-        <v>130</v>
+        <v>127</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
feature: updated for answer to reviewers
</commit_message>
<xml_diff>
--- a/tables/combination_drugs.xlsx
+++ b/tables/combination_drugs.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="24701"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Vincent\Documents\pmx-models-atb-review\tables\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\UMR-1070\Documents\Vincent\Github\pmx-models-atb-review\tables\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{68DC73D1-FFE9-4079-9397-C5398C86DCA2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1116" yWindow="1116" windowWidth="17280" windowHeight="8964" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1110" yWindow="1110" windowWidth="17280" windowHeight="8970"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="425" uniqueCount="210">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="425" uniqueCount="207">
   <si>
     <t>Drugs</t>
   </si>
@@ -343,9 +342,6 @@
     <t>Pseudomonas aeruginosa, 6 strains</t>
   </si>
   <si>
-    <t>subpopualations, NA</t>
-  </si>
-  <si>
     <t>https://www.ncbi.nlm.nih.gov/pmc/articles/PMC4862466/pdf/zac2870.pdf</t>
   </si>
   <si>
@@ -355,9 +351,6 @@
     <t>Emax, death, no, meropenem, NA, NA</t>
   </si>
   <si>
-    <t>subpopualations, NA;other, signal molecules</t>
-  </si>
-  <si>
     <t>https://academic.oup.com/jac/article/72/1/153/2643127</t>
   </si>
   <si>
@@ -487,9 +480,6 @@
     <t>patients, experimental setup</t>
   </si>
   <si>
-    <t>Escherichia coli</t>
-  </si>
-  <si>
     <t>Garrett</t>
   </si>
   <si>
@@ -499,15 +489,9 @@
     <t>linear, death, no, tetracycline, NA, NA;linear, death, no, chloramphenicol, NA, NA</t>
   </si>
   <si>
-    <t>Pseudomonas aeruginosa</t>
-  </si>
-  <si>
     <t>Smith</t>
   </si>
   <si>
-    <t>Acinetobacter baumannii</t>
-  </si>
-  <si>
     <t>sEmax, death, no, meropenem, NA, NA;linear, death, no, polymyxin B, NA, NA</t>
   </si>
   <si>
@@ -650,12 +634,18 @@
   </si>
   <si>
     <t>critically ill with ARC, simulations;critically ill with arc, experimental setup</t>
+  </si>
+  <si>
+    <t>subpopulaations, NA</t>
+  </si>
+  <si>
+    <t>subpopulaations, NA;other, signal molecules</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -792,23 +782,6 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
@@ -844,23 +817,6 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -1036,16 +992,16 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:O41"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="G1" workbookViewId="0">
-      <selection activeCell="N21" sqref="N21"/>
+    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
+      <selection activeCell="B42" sqref="B42"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:15" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:15" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1092,7 +1048,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>15</v>
       </c>
@@ -1112,25 +1068,25 @@
         <v>18</v>
       </c>
       <c r="G2" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="H2" t="s">
         <v>19</v>
       </c>
       <c r="I2" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="J2" t="s">
         <v>20</v>
       </c>
       <c r="K2" t="s">
-        <v>164</v>
+        <v>159</v>
       </c>
       <c r="L2" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.3">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>21</v>
       </c>
@@ -1150,25 +1106,25 @@
         <v>24</v>
       </c>
       <c r="G3" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="H3" t="s">
         <v>19</v>
       </c>
       <c r="I3" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="J3" t="s">
         <v>20</v>
       </c>
       <c r="K3" t="s">
-        <v>188</v>
+        <v>183</v>
       </c>
       <c r="L3" t="s">
-        <v>118</v>
-      </c>
-    </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.3">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>25</v>
       </c>
@@ -1188,25 +1144,25 @@
         <v>24</v>
       </c>
       <c r="G4" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="H4" t="s">
         <v>19</v>
       </c>
       <c r="I4" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="J4" t="s">
         <v>20</v>
       </c>
       <c r="K4" t="s">
-        <v>189</v>
+        <v>184</v>
       </c>
       <c r="L4" t="s">
-        <v>118</v>
-      </c>
-    </row>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.3">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>27</v>
       </c>
@@ -1226,7 +1182,7 @@
         <v>30</v>
       </c>
       <c r="G5" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="H5" t="s">
         <v>31</v>
@@ -1238,15 +1194,15 @@
         <v>20</v>
       </c>
       <c r="K5" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="L5" t="s">
-        <v>209</v>
-      </c>
-    </row>
-    <row r="6" spans="1:15" x14ac:dyDescent="0.3">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="6" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>168</v>
+        <v>163</v>
       </c>
       <c r="B6" t="s">
         <v>33</v>
@@ -1264,30 +1220,30 @@
         <v>18</v>
       </c>
       <c r="G6" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="H6" t="s">
         <v>31</v>
       </c>
       <c r="I6" t="s">
-        <v>169</v>
+        <v>164</v>
       </c>
       <c r="J6" t="s">
         <v>20</v>
       </c>
       <c r="K6" t="s">
-        <v>208</v>
+        <v>203</v>
       </c>
       <c r="L6" t="s">
-        <v>163</v>
+        <v>158</v>
       </c>
       <c r="M6" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="7" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>170</v>
+        <v>165</v>
       </c>
       <c r="B7" t="s">
         <v>33</v>
@@ -1305,30 +1261,30 @@
         <v>24</v>
       </c>
       <c r="G7" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="H7" t="s">
         <v>37</v>
       </c>
       <c r="I7" t="s">
-        <v>204</v>
+        <v>199</v>
       </c>
       <c r="J7" t="s">
         <v>38</v>
       </c>
       <c r="K7" t="s">
-        <v>205</v>
+        <v>200</v>
       </c>
       <c r="L7" t="s">
-        <v>163</v>
+        <v>158</v>
       </c>
       <c r="M7" t="s">
-        <v>135</v>
-      </c>
-    </row>
-    <row r="8" spans="1:15" x14ac:dyDescent="0.3">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="8" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>170</v>
+        <v>165</v>
       </c>
       <c r="B8" t="s">
         <v>39</v>
@@ -1346,28 +1302,28 @@
         <v>24</v>
       </c>
       <c r="G8" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="H8" t="s">
         <v>19</v>
       </c>
       <c r="I8" t="s">
-        <v>171</v>
+        <v>166</v>
       </c>
       <c r="J8" t="s">
         <v>41</v>
       </c>
       <c r="K8" t="s">
-        <v>190</v>
+        <v>185</v>
       </c>
       <c r="L8" t="s">
-        <v>163</v>
+        <v>158</v>
       </c>
       <c r="N8" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="9" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>43</v>
       </c>
@@ -1375,7 +1331,7 @@
         <v>44</v>
       </c>
       <c r="C9" t="s">
-        <v>202</v>
+        <v>197</v>
       </c>
       <c r="D9">
         <v>2020</v>
@@ -1387,25 +1343,25 @@
         <v>24</v>
       </c>
       <c r="G9" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="H9" t="s">
         <v>37</v>
       </c>
       <c r="I9" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="J9" t="s">
-        <v>203</v>
+        <v>198</v>
       </c>
       <c r="K9" t="s">
-        <v>191</v>
+        <v>186</v>
       </c>
       <c r="L9" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="10" spans="1:15" x14ac:dyDescent="0.3">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="10" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>45</v>
       </c>
@@ -1425,25 +1381,25 @@
         <v>24</v>
       </c>
       <c r="G10" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="H10" t="s">
         <v>31</v>
       </c>
       <c r="I10" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="J10" t="s">
         <v>20</v>
       </c>
       <c r="K10" t="s">
-        <v>192</v>
+        <v>187</v>
       </c>
       <c r="L10" t="s">
-        <v>163</v>
-      </c>
-    </row>
-    <row r="11" spans="1:15" x14ac:dyDescent="0.3">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="11" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>48</v>
       </c>
@@ -1463,25 +1419,25 @@
         <v>51</v>
       </c>
       <c r="G11" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="H11" t="s">
         <v>37</v>
       </c>
       <c r="I11" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="J11" t="s">
         <v>38</v>
       </c>
       <c r="K11" t="s">
-        <v>193</v>
+        <v>188</v>
       </c>
       <c r="L11" t="s">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="12" spans="1:15" x14ac:dyDescent="0.3">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="12" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>52</v>
       </c>
@@ -1501,25 +1457,25 @@
         <v>24</v>
       </c>
       <c r="G12" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="H12" t="s">
         <v>19</v>
       </c>
       <c r="I12" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="J12" t="s">
         <v>20</v>
       </c>
       <c r="K12" t="s">
-        <v>201</v>
+        <v>196</v>
       </c>
       <c r="L12" t="s">
-        <v>121</v>
-      </c>
-    </row>
-    <row r="13" spans="1:15" x14ac:dyDescent="0.3">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="13" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>55</v>
       </c>
@@ -1539,13 +1495,13 @@
         <v>58</v>
       </c>
       <c r="G13" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="H13" t="s">
         <v>19</v>
       </c>
       <c r="I13" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="J13" t="s">
         <v>38</v>
@@ -1554,12 +1510,12 @@
         <v>59</v>
       </c>
       <c r="L13" t="s">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="14" spans="1:15" x14ac:dyDescent="0.3">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="14" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>172</v>
+        <v>167</v>
       </c>
       <c r="B14" t="s">
         <v>60</v>
@@ -1577,25 +1533,25 @@
         <v>24</v>
       </c>
       <c r="G14" t="s">
-        <v>200</v>
+        <v>195</v>
       </c>
       <c r="H14" t="s">
         <v>19</v>
       </c>
       <c r="I14" t="s">
-        <v>173</v>
+        <v>168</v>
       </c>
       <c r="J14" t="s">
         <v>20</v>
       </c>
       <c r="K14" t="s">
-        <v>194</v>
+        <v>189</v>
       </c>
       <c r="L14" t="s">
-        <v>163</v>
-      </c>
-    </row>
-    <row r="15" spans="1:15" x14ac:dyDescent="0.3">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="15" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>62</v>
       </c>
@@ -1615,28 +1571,28 @@
         <v>24</v>
       </c>
       <c r="G15" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="H15" t="s">
         <v>19</v>
       </c>
       <c r="I15" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="J15" t="s">
         <v>38</v>
       </c>
       <c r="K15" t="s">
-        <v>206</v>
+        <v>201</v>
       </c>
       <c r="L15" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="N15" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="16" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>66</v>
       </c>
@@ -1656,25 +1612,25 @@
         <v>18</v>
       </c>
       <c r="G16" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="H16" t="s">
         <v>19</v>
       </c>
       <c r="I16" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="J16" t="s">
         <v>20</v>
       </c>
       <c r="K16" t="s">
-        <v>164</v>
+        <v>159</v>
       </c>
       <c r="L16" t="s">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="17" spans="1:13" x14ac:dyDescent="0.3">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="17" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>27</v>
       </c>
@@ -1694,27 +1650,27 @@
         <v>30</v>
       </c>
       <c r="G17" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="H17" t="s">
         <v>69</v>
       </c>
       <c r="I17" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="J17" t="s">
         <v>20</v>
       </c>
       <c r="K17" t="s">
-        <v>195</v>
+        <v>190</v>
       </c>
       <c r="L17" t="s">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="18" spans="1:13" x14ac:dyDescent="0.3">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="18" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>174</v>
+        <v>169</v>
       </c>
       <c r="B18" t="s">
         <v>28</v>
@@ -1732,25 +1688,25 @@
         <v>70</v>
       </c>
       <c r="G18" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="H18" t="s">
         <v>69</v>
       </c>
       <c r="I18" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="J18" t="s">
         <v>20</v>
       </c>
       <c r="K18" t="s">
-        <v>196</v>
+        <v>191</v>
       </c>
       <c r="L18" t="s">
-        <v>125</v>
-      </c>
-    </row>
-    <row r="19" spans="1:13" x14ac:dyDescent="0.3">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="19" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>71</v>
       </c>
@@ -1770,25 +1726,25 @@
         <v>30</v>
       </c>
       <c r="G19" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="H19" t="s">
         <v>69</v>
       </c>
       <c r="I19" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="J19" t="s">
         <v>20</v>
       </c>
       <c r="K19" t="s">
-        <v>197</v>
+        <v>192</v>
       </c>
       <c r="L19" t="s">
-        <v>126</v>
-      </c>
-    </row>
-    <row r="20" spans="1:13" x14ac:dyDescent="0.3">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="20" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>73</v>
       </c>
@@ -1808,25 +1764,25 @@
         <v>30</v>
       </c>
       <c r="G20" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="H20" t="s">
         <v>69</v>
       </c>
       <c r="I20" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="J20" t="s">
         <v>20</v>
       </c>
       <c r="K20" t="s">
-        <v>198</v>
+        <v>193</v>
       </c>
       <c r="L20" t="s">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="21" spans="1:13" x14ac:dyDescent="0.3">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="21" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>43</v>
       </c>
@@ -1846,25 +1802,25 @@
         <v>24</v>
       </c>
       <c r="G21" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="H21" t="s">
         <v>19</v>
       </c>
       <c r="I21" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="J21" t="s">
         <v>20</v>
       </c>
       <c r="K21" t="s">
-        <v>179</v>
+        <v>174</v>
       </c>
       <c r="L21" t="s">
-        <v>154</v>
-      </c>
-    </row>
-    <row r="22" spans="1:13" x14ac:dyDescent="0.3">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="22" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>77</v>
       </c>
@@ -1884,25 +1840,25 @@
         <v>18</v>
       </c>
       <c r="G22" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="H22" t="s">
-        <v>186</v>
+        <v>181</v>
       </c>
       <c r="I22" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="J22" t="s">
         <v>20</v>
       </c>
       <c r="K22" t="s">
-        <v>187</v>
+        <v>182</v>
       </c>
       <c r="L22" t="s">
-        <v>127</v>
-      </c>
-    </row>
-    <row r="23" spans="1:13" x14ac:dyDescent="0.3">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="23" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>77</v>
       </c>
@@ -1919,31 +1875,31 @@
         <v>28993331</v>
       </c>
       <c r="F23" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="G23" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="H23" t="s">
         <v>31</v>
       </c>
       <c r="I23" t="s">
-        <v>182</v>
+        <v>177</v>
       </c>
       <c r="J23" t="s">
         <v>20</v>
       </c>
       <c r="K23" t="s">
-        <v>199</v>
+        <v>194</v>
       </c>
       <c r="L23" t="s">
-        <v>163</v>
+        <v>158</v>
       </c>
       <c r="M23" t="s">
         <v>78</v>
       </c>
     </row>
-    <row r="24" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>79</v>
       </c>
@@ -1963,25 +1919,25 @@
         <v>24</v>
       </c>
       <c r="G24" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="H24" t="s">
         <v>31</v>
       </c>
       <c r="I24" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="J24" t="s">
         <v>20</v>
       </c>
       <c r="K24" t="s">
-        <v>199</v>
+        <v>194</v>
       </c>
       <c r="L24" t="s">
-        <v>163</v>
-      </c>
-    </row>
-    <row r="25" spans="1:13" x14ac:dyDescent="0.3">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="25" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>80</v>
       </c>
@@ -2001,25 +1957,25 @@
         <v>24</v>
       </c>
       <c r="G25" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="H25" t="s">
         <v>83</v>
       </c>
       <c r="I25" t="s">
-        <v>184</v>
+        <v>179</v>
       </c>
       <c r="J25" t="s">
         <v>38</v>
       </c>
       <c r="K25" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="L25" t="s">
-        <v>183</v>
-      </c>
-    </row>
-    <row r="26" spans="1:13" x14ac:dyDescent="0.3">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="26" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>52</v>
       </c>
@@ -2039,25 +1995,25 @@
         <v>24</v>
       </c>
       <c r="G26" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="H26" t="s">
         <v>37</v>
       </c>
       <c r="I26" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="J26" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="K26" t="s">
-        <v>185</v>
+        <v>180</v>
       </c>
       <c r="L26" t="s">
-        <v>163</v>
-      </c>
-    </row>
-    <row r="27" spans="1:13" x14ac:dyDescent="0.3">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="27" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>85</v>
       </c>
@@ -2077,27 +2033,27 @@
         <v>24</v>
       </c>
       <c r="G27" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="H27" t="s">
         <v>31</v>
       </c>
       <c r="I27" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="J27" t="s">
         <v>86</v>
       </c>
       <c r="K27" t="s">
-        <v>207</v>
+        <v>202</v>
       </c>
       <c r="L27" t="s">
-        <v>163</v>
-      </c>
-    </row>
-    <row r="28" spans="1:13" x14ac:dyDescent="0.3">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="28" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>166</v>
+        <v>161</v>
       </c>
       <c r="B28" t="s">
         <v>22</v>
@@ -2115,28 +2071,28 @@
         <v>30</v>
       </c>
       <c r="G28" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="H28" t="s">
         <v>31</v>
       </c>
       <c r="I28" t="s">
-        <v>175</v>
+        <v>170</v>
       </c>
       <c r="J28" t="s">
         <v>20</v>
       </c>
       <c r="K28" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="L28" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="M28" t="s">
         <v>88</v>
       </c>
     </row>
-    <row r="29" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>55</v>
       </c>
@@ -2156,13 +2112,13 @@
         <v>24</v>
       </c>
       <c r="G29" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="H29" t="s">
         <v>37</v>
       </c>
       <c r="I29" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="J29" t="s">
         <v>90</v>
@@ -2171,10 +2127,10 @@
         <v>59</v>
       </c>
       <c r="L29" t="s">
-        <v>128</v>
-      </c>
-    </row>
-    <row r="30" spans="1:13" x14ac:dyDescent="0.3">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="30" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>66</v>
       </c>
@@ -2194,25 +2150,25 @@
         <v>18</v>
       </c>
       <c r="G30" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="H30" t="s">
         <v>19</v>
       </c>
       <c r="I30" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="J30" t="s">
         <v>20</v>
       </c>
       <c r="K30" t="s">
-        <v>164</v>
+        <v>159</v>
       </c>
       <c r="L30" t="s">
-        <v>129</v>
-      </c>
-    </row>
-    <row r="31" spans="1:13" x14ac:dyDescent="0.3">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="31" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>93</v>
       </c>
@@ -2232,28 +2188,28 @@
         <v>18</v>
       </c>
       <c r="G31" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="H31" t="s">
         <v>31</v>
       </c>
       <c r="I31" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="J31" t="s">
         <v>20</v>
       </c>
       <c r="K31" t="s">
-        <v>180</v>
+        <v>175</v>
       </c>
       <c r="L31" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="M31" t="s">
         <v>95</v>
       </c>
     </row>
-    <row r="32" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>96</v>
       </c>
@@ -2273,25 +2229,25 @@
         <v>24</v>
       </c>
       <c r="G32" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="H32" t="s">
         <v>31</v>
       </c>
       <c r="I32" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="J32" t="s">
         <v>86</v>
       </c>
       <c r="K32" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="L32" t="s">
-        <v>128</v>
-      </c>
-    </row>
-    <row r="33" spans="1:14" x14ac:dyDescent="0.3">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="33" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>97</v>
       </c>
@@ -2311,25 +2267,25 @@
         <v>58</v>
       </c>
       <c r="G33" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="H33" t="s">
         <v>37</v>
       </c>
       <c r="I33" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="J33" t="s">
         <v>38</v>
       </c>
       <c r="K33" t="s">
-        <v>164</v>
+        <v>159</v>
       </c>
       <c r="L33" t="s">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="34" spans="1:14" x14ac:dyDescent="0.3">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="34" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>100</v>
       </c>
@@ -2346,33 +2302,33 @@
         <v>25362196</v>
       </c>
       <c r="F34" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="G34" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="H34" t="s">
         <v>19</v>
       </c>
       <c r="I34" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="J34" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="K34" t="s">
-        <v>164</v>
+        <v>159</v>
       </c>
       <c r="L34" t="s">
-        <v>163</v>
+        <v>158</v>
       </c>
       <c r="M34" t="s">
         <v>102</v>
       </c>
     </row>
-    <row r="35" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>165</v>
+        <v>160</v>
       </c>
       <c r="B35" t="s">
         <v>81</v>
@@ -2390,27 +2346,27 @@
         <v>24</v>
       </c>
       <c r="G35" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="H35" t="s">
         <v>31</v>
       </c>
       <c r="I35" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="J35" t="s">
         <v>20</v>
       </c>
       <c r="K35" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="L35" t="s">
-        <v>163</v>
-      </c>
-    </row>
-    <row r="36" spans="1:14" x14ac:dyDescent="0.3">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="36" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="B36" t="s">
         <v>103</v>
@@ -2428,27 +2384,27 @@
         <v>24</v>
       </c>
       <c r="G36" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="H36" t="s">
         <v>19</v>
       </c>
       <c r="I36" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="J36" t="s">
         <v>105</v>
       </c>
       <c r="K36" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="L36" t="s">
-        <v>163</v>
-      </c>
-    </row>
-    <row r="37" spans="1:14" x14ac:dyDescent="0.3">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="37" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>166</v>
+        <v>161</v>
       </c>
       <c r="B37" t="s">
         <v>106</v>
@@ -2466,36 +2422,36 @@
         <v>24</v>
       </c>
       <c r="G37" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="H37" t="s">
         <v>31</v>
       </c>
       <c r="I37" t="s">
-        <v>176</v>
+        <v>171</v>
       </c>
       <c r="J37" t="s">
+        <v>205</v>
+      </c>
+      <c r="K37" t="s">
+        <v>162</v>
+      </c>
+      <c r="L37" t="s">
+        <v>126</v>
+      </c>
+      <c r="N37" t="s">
         <v>107</v>
       </c>
-      <c r="K37" t="s">
-        <v>167</v>
-      </c>
-      <c r="L37" t="s">
-        <v>128</v>
-      </c>
-      <c r="N37" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="38" spans="1:14" x14ac:dyDescent="0.3">
+    </row>
+    <row r="38" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>177</v>
+        <v>172</v>
       </c>
       <c r="B38" t="s">
         <v>56</v>
       </c>
       <c r="C38" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="D38">
         <v>2017</v>
@@ -2507,36 +2463,36 @@
         <v>30</v>
       </c>
       <c r="G38" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="H38" t="s">
         <v>31</v>
       </c>
       <c r="I38" t="s">
+        <v>109</v>
+      </c>
+      <c r="J38" t="s">
+        <v>206</v>
+      </c>
+      <c r="K38" t="s">
+        <v>173</v>
+      </c>
+      <c r="L38" t="s">
+        <v>125</v>
+      </c>
+      <c r="N38" t="s">
         <v>110</v>
       </c>
-      <c r="J38" t="s">
-        <v>111</v>
-      </c>
-      <c r="K38" t="s">
-        <v>178</v>
-      </c>
-      <c r="L38" t="s">
-        <v>127</v>
-      </c>
-      <c r="N38" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="39" spans="1:14" x14ac:dyDescent="0.3">
+    </row>
+    <row r="39" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>157</v>
+        <v>154</v>
       </c>
       <c r="B39" t="s">
-        <v>155</v>
+        <v>91</v>
       </c>
       <c r="C39" t="s">
-        <v>156</v>
+        <v>153</v>
       </c>
       <c r="D39">
         <v>1963</v>
@@ -2548,30 +2504,30 @@
         <v>24</v>
       </c>
       <c r="G39" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="H39" t="s">
         <v>19</v>
       </c>
       <c r="I39" t="s">
+        <v>155</v>
+      </c>
+      <c r="J39" t="s">
+        <v>112</v>
+      </c>
+      <c r="K39" t="s">
+        <v>113</v>
+      </c>
+      <c r="L39" t="s">
         <v>158</v>
       </c>
-      <c r="J39" t="s">
-        <v>114</v>
-      </c>
-      <c r="K39" t="s">
-        <v>115</v>
-      </c>
-      <c r="L39" t="s">
-        <v>163</v>
-      </c>
-    </row>
-    <row r="40" spans="1:14" x14ac:dyDescent="0.3">
+    </row>
+    <row r="40" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>73</v>
       </c>
       <c r="B40" t="s">
-        <v>159</v>
+        <v>74</v>
       </c>
       <c r="C40" t="s">
         <v>72</v>
@@ -2586,33 +2542,33 @@
         <v>30</v>
       </c>
       <c r="G40" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="H40" t="s">
         <v>69</v>
       </c>
       <c r="I40" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="J40" t="s">
         <v>20</v>
       </c>
       <c r="K40" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="L40" t="s">
-        <v>126</v>
-      </c>
-    </row>
-    <row r="41" spans="1:14" x14ac:dyDescent="0.3">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="41" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>177</v>
+        <v>172</v>
       </c>
       <c r="B41" t="s">
-        <v>161</v>
+        <v>39</v>
       </c>
       <c r="C41" t="s">
-        <v>160</v>
+        <v>156</v>
       </c>
       <c r="D41">
         <v>2020</v>
@@ -2624,22 +2580,22 @@
         <v>18</v>
       </c>
       <c r="G41" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="H41" t="s">
         <v>31</v>
       </c>
       <c r="I41" t="s">
-        <v>162</v>
+        <v>157</v>
       </c>
       <c r="J41" t="s">
         <v>20</v>
       </c>
       <c r="K41" t="s">
-        <v>181</v>
+        <v>176</v>
       </c>
       <c r="L41" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
fix: more corrections to the table and underlying data
</commit_message>
<xml_diff>
--- a/tables/combination_drugs.xlsx
+++ b/tables/combination_drugs.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="425" uniqueCount="207">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="425" uniqueCount="205">
   <si>
     <t>Drugs</t>
   </si>
@@ -634,12 +634,6 @@
   </si>
   <si>
     <t>critically ill with ARC, simulations;critically ill with arc, experimental setup</t>
-  </si>
-  <si>
-    <t>subpopulaations, NA</t>
-  </si>
-  <si>
-    <t>subpopulaations, NA;other, signal molecules</t>
   </si>
 </sst>
 </file>
@@ -996,7 +990,7 @@
   <dimension ref="A1:O41"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
-      <selection activeCell="B42" sqref="B42"/>
+      <selection activeCell="J38" sqref="J38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2431,7 +2425,7 @@
         <v>171</v>
       </c>
       <c r="J37" t="s">
-        <v>205</v>
+        <v>20</v>
       </c>
       <c r="K37" t="s">
         <v>162</v>
@@ -2472,7 +2466,7 @@
         <v>109</v>
       </c>
       <c r="J38" t="s">
-        <v>206</v>
+        <v>86</v>
       </c>
       <c r="K38" t="s">
         <v>173</v>

</xml_diff>